<commit_message>
add config file handling
</commit_message>
<xml_diff>
--- a/Auslastung.xlsx
+++ b/Auslastung.xlsx
@@ -2252,14 +2252,30 @@
       <c r="AE2" s="1" t="str">
         <v>22.07-28.07.19</v>
       </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="AF2" s="1" t="str">
+        <v>29.07-04.08.19</v>
+      </c>
+      <c r="AG2" s="1" t="str">
+        <v>05.08-11.08.19</v>
+      </c>
+      <c r="AH2" s="1" t="str">
+        <v>12.08-18.08.19</v>
+      </c>
+      <c r="AI2" s="1" t="str">
+        <v>19.08-25.08.19</v>
+      </c>
+      <c r="AJ2" s="1" t="str">
+        <v>26.08-01.09.19</v>
+      </c>
+      <c r="AK2" s="1" t="str">
+        <v>02.09-08.09.19</v>
+      </c>
+      <c r="AL2" s="1" t="str">
+        <v>09.09-15.09.19</v>
+      </c>
+      <c r="AM2" s="1" t="str">
+        <v>16.09-22.09.19</v>
+      </c>
       <c r="AN2" s="18"/>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
@@ -2448,7 +2464,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="AM4" t="str"/>
+    </row>
     <row ht="34" r="5" spans="1:54">
       <c r="A5" s="2" t="s">
         <v>2</v>
@@ -2769,7 +2787,9 @@
       </c>
       <c r="BB6" s="3"/>
     </row>
-    <row r="7"/>
+    <row r="7">
+      <c r="AM7" t="str"/>
+    </row>
     <row ht="25" r="8" spans="1:54">
       <c r="A8" s="5" t="s">
         <v>104</v>
@@ -2869,9 +2889,15 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="6"/>
       <c r="AJ8" s="6"/>
-      <c r="AK8" s="6"/>
-      <c r="AL8" s="6"/>
-      <c r="AM8" s="19"/>
+      <c r="AK8" s="6">
+        <v>34.50</v>
+      </c>
+      <c r="AL8" s="6">
+        <v>34.50</v>
+      </c>
+      <c r="AM8" s="19">
+        <v>34.50</v>
+      </c>
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
@@ -2988,9 +3014,15 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="6"/>
       <c r="AJ9" s="6"/>
-      <c r="AK9" s="6"/>
-      <c r="AL9" s="6"/>
-      <c r="AM9" s="19"/>
+      <c r="AK9" s="6">
+        <v>8.50</v>
+      </c>
+      <c r="AL9" s="6">
+        <v>8.50</v>
+      </c>
+      <c r="AM9" s="19">
+        <v>8.50</v>
+      </c>
       <c r="AN9" s="19"/>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
@@ -3266,7 +3298,7 @@
       <c r="AJ11" s="6"/>
       <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="19"/>
+      <c r="AM11" s="19" t="str"/>
       <c r="AN11" s="19"/>
       <c r="AO11" s="19"/>
       <c r="AP11" s="19"/>
@@ -3378,9 +3410,15 @@
       <c r="AH12" s="10"/>
       <c r="AI12" s="10"/>
       <c r="AJ12" s="10"/>
-      <c r="AK12" s="10"/>
-      <c r="AL12" s="10"/>
-      <c r="AM12" s="20"/>
+      <c r="AK12" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="AL12" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="AM12" s="20">
+        <v>1.25</v>
+      </c>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20"/>
@@ -3465,9 +3503,15 @@
       <c r="AH13" s="10"/>
       <c r="AI13" s="10"/>
       <c r="AJ13" s="10"/>
-      <c r="AK13" s="10"/>
-      <c r="AL13" s="10"/>
-      <c r="AM13" s="20"/>
+      <c r="AK13" s="10">
+        <v>11.75</v>
+      </c>
+      <c r="AL13" s="10">
+        <v>11.75</v>
+      </c>
+      <c r="AM13" s="20">
+        <v>11.75</v>
+      </c>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
@@ -3588,7 +3632,9 @@
       <c r="AJ14" s="10"/>
       <c r="AK14" s="10"/>
       <c r="AL14" s="10"/>
-      <c r="AM14" s="20"/>
+      <c r="AM14" s="20">
+        <v>13.50</v>
+      </c>
       <c r="AN14" s="38"/>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
@@ -3707,9 +3753,15 @@
       <c r="AH15" s="10"/>
       <c r="AI15" s="10"/>
       <c r="AJ15" s="10"/>
-      <c r="AK15" s="10"/>
-      <c r="AL15" s="10"/>
-      <c r="AM15" s="20"/>
+      <c r="AK15" s="10">
+        <v>17.50</v>
+      </c>
+      <c r="AL15" s="10">
+        <v>17.50</v>
+      </c>
+      <c r="AM15" s="20">
+        <v>17.50</v>
+      </c>
       <c r="AN15" s="38"/>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
@@ -3828,7 +3880,9 @@
       <c r="AJ16" s="10"/>
       <c r="AK16" s="10"/>
       <c r="AL16" s="10"/>
-      <c r="AM16" s="20"/>
+      <c r="AM16" s="20">
+        <v>13.25</v>
+      </c>
       <c r="AN16" s="38"/>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
@@ -3947,9 +4001,15 @@
       <c r="AH17" s="10"/>
       <c r="AI17" s="10"/>
       <c r="AJ17" s="10"/>
-      <c r="AK17" s="10"/>
-      <c r="AL17" s="10"/>
-      <c r="AM17" s="20"/>
+      <c r="AK17" s="10">
+        <v>19.50</v>
+      </c>
+      <c r="AL17" s="10">
+        <v>19.50</v>
+      </c>
+      <c r="AM17" s="20">
+        <v>19.50</v>
+      </c>
       <c r="AN17" s="38"/>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20"/>
@@ -4046,7 +4106,7 @@
       <c r="AJ18" s="10"/>
       <c r="AK18" s="10"/>
       <c r="AL18" s="10"/>
-      <c r="AM18" s="20"/>
+      <c r="AM18" s="20" t="str"/>
       <c r="AN18" s="38"/>
       <c r="AO18" s="20"/>
       <c r="AP18" s="20"/>
@@ -4165,9 +4225,15 @@
       <c r="AH19" s="10"/>
       <c r="AI19" s="10"/>
       <c r="AJ19" s="10"/>
-      <c r="AK19" s="10"/>
-      <c r="AL19" s="10"/>
-      <c r="AM19" s="20"/>
+      <c r="AK19" s="10">
+        <v>20.50</v>
+      </c>
+      <c r="AL19" s="10">
+        <v>20.50</v>
+      </c>
+      <c r="AM19" s="20">
+        <v>20.50</v>
+      </c>
       <c r="AN19" s="38"/>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
@@ -4284,9 +4350,15 @@
       <c r="AH20" s="10"/>
       <c r="AI20" s="10"/>
       <c r="AJ20" s="10"/>
-      <c r="AK20" s="10"/>
-      <c r="AL20" s="10"/>
-      <c r="AM20" s="37"/>
+      <c r="AK20" s="10">
+        <v>5.75</v>
+      </c>
+      <c r="AL20" s="10">
+        <v>5.75</v>
+      </c>
+      <c r="AM20" s="37">
+        <v>5.75</v>
+      </c>
       <c r="AN20" s="37"/>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
@@ -4405,9 +4477,15 @@
       <c r="AH21" s="35"/>
       <c r="AI21" s="35"/>
       <c r="AJ21" s="35"/>
-      <c r="AK21" s="35"/>
-      <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
+      <c r="AK21" s="35">
+        <v>25.00</v>
+      </c>
+      <c r="AL21" s="35">
+        <v>25.00</v>
+      </c>
+      <c r="AM21" s="35">
+        <v>25.00</v>
+      </c>
       <c r="AN21" s="35"/>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
@@ -4526,9 +4604,15 @@
       <c r="AH22" s="35"/>
       <c r="AI22" s="35"/>
       <c r="AJ22" s="35"/>
-      <c r="AK22" s="35"/>
-      <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
+      <c r="AK22" s="35">
+        <v>5.75</v>
+      </c>
+      <c r="AL22" s="35">
+        <v>5.75</v>
+      </c>
+      <c r="AM22" s="35">
+        <v>5.75</v>
+      </c>
       <c r="AN22" s="35"/>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
@@ -4804,7 +4888,7 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
-      <c r="AM24" s="19"/>
+      <c r="AM24" s="19" t="str"/>
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
       <c r="AP24" s="19"/>
@@ -4918,9 +5002,15 @@
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
       <c r="AJ25" s="6"/>
-      <c r="AK25" s="6"/>
-      <c r="AL25" s="6"/>
-      <c r="AM25" s="19"/>
+      <c r="AK25" s="6">
+        <v>17.00</v>
+      </c>
+      <c r="AL25" s="6">
+        <v>17.00</v>
+      </c>
+      <c r="AM25" s="19">
+        <v>17.00</v>
+      </c>
       <c r="AN25" s="19"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
@@ -5033,9 +5123,15 @@
       <c r="AH26" s="10"/>
       <c r="AI26" s="10"/>
       <c r="AJ26" s="10"/>
-      <c r="AK26" s="10"/>
-      <c r="AL26" s="10"/>
-      <c r="AM26" s="20"/>
+      <c r="AK26" s="10">
+        <v>13.00</v>
+      </c>
+      <c r="AL26" s="10">
+        <v>13.00</v>
+      </c>
+      <c r="AM26" s="20">
+        <v>13.00</v>
+      </c>
       <c r="AN26" s="38"/>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
@@ -5154,9 +5250,15 @@
       <c r="AH27" s="10"/>
       <c r="AI27" s="10"/>
       <c r="AJ27" s="10"/>
-      <c r="AK27" s="10"/>
-      <c r="AL27" s="10"/>
-      <c r="AM27" s="20"/>
+      <c r="AK27" s="10">
+        <v>29.00</v>
+      </c>
+      <c r="AL27" s="10">
+        <v>29.00</v>
+      </c>
+      <c r="AM27" s="20">
+        <v>29.00</v>
+      </c>
       <c r="AN27" s="38"/>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
@@ -5269,7 +5371,9 @@
       <c r="AJ28" s="10"/>
       <c r="AK28" s="10"/>
       <c r="AL28" s="10"/>
-      <c r="AM28" s="20"/>
+      <c r="AM28" s="20">
+        <v>4.75</v>
+      </c>
       <c r="AN28" s="38"/>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
@@ -5384,9 +5488,15 @@
       <c r="AH29" s="10"/>
       <c r="AI29" s="10"/>
       <c r="AJ29" s="10"/>
-      <c r="AK29" s="10"/>
-      <c r="AL29" s="10"/>
-      <c r="AM29" s="20"/>
+      <c r="AK29" s="10">
+        <v>19.75</v>
+      </c>
+      <c r="AL29" s="10">
+        <v>19.75</v>
+      </c>
+      <c r="AM29" s="20">
+        <v>19.75</v>
+      </c>
       <c r="AN29" s="38"/>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
@@ -5505,9 +5615,15 @@
       <c r="AH30" s="10"/>
       <c r="AI30" s="10"/>
       <c r="AJ30" s="10"/>
-      <c r="AK30" s="10"/>
-      <c r="AL30" s="10"/>
-      <c r="AM30" s="20"/>
+      <c r="AK30" s="10">
+        <v>21.00</v>
+      </c>
+      <c r="AL30" s="10">
+        <v>21.00</v>
+      </c>
+      <c r="AM30" s="20">
+        <v>21.00</v>
+      </c>
       <c r="AN30" s="38"/>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
@@ -5622,7 +5738,7 @@
       <c r="AJ31" s="10"/>
       <c r="AK31" s="10"/>
       <c r="AL31" s="10"/>
-      <c r="AM31" s="20"/>
+      <c r="AM31" s="20" t="str"/>
       <c r="AN31" s="38"/>
       <c r="AO31" s="20"/>
       <c r="AP31" s="20"/>
@@ -5741,9 +5857,15 @@
       <c r="AH32" s="10"/>
       <c r="AI32" s="10"/>
       <c r="AJ32" s="10"/>
-      <c r="AK32" s="10"/>
-      <c r="AL32" s="10"/>
-      <c r="AM32" s="20"/>
+      <c r="AK32" s="10">
+        <v>20.50</v>
+      </c>
+      <c r="AL32" s="10">
+        <v>20.50</v>
+      </c>
+      <c r="AM32" s="20">
+        <v>20.50</v>
+      </c>
       <c r="AN32" s="38"/>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
@@ -5862,9 +5984,15 @@
       <c r="AH33" s="10"/>
       <c r="AI33" s="10"/>
       <c r="AJ33" s="10"/>
-      <c r="AK33" s="10"/>
-      <c r="AL33" s="10"/>
-      <c r="AM33" s="20"/>
+      <c r="AK33" s="10">
+        <v>14.25</v>
+      </c>
+      <c r="AL33" s="10">
+        <v>14.25</v>
+      </c>
+      <c r="AM33" s="20">
+        <v>14.25</v>
+      </c>
       <c r="AN33" s="38"/>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
@@ -5983,9 +6111,15 @@
       <c r="AH34" s="35"/>
       <c r="AI34" s="35"/>
       <c r="AJ34" s="35"/>
-      <c r="AK34" s="35"/>
-      <c r="AL34" s="35"/>
-      <c r="AM34" s="35"/>
+      <c r="AK34" s="35">
+        <v>39.00</v>
+      </c>
+      <c r="AL34" s="35">
+        <v>39.00</v>
+      </c>
+      <c r="AM34" s="35">
+        <v>39.00</v>
+      </c>
       <c r="AN34" s="35"/>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
@@ -6104,9 +6238,15 @@
       <c r="AH35" s="35"/>
       <c r="AI35" s="35"/>
       <c r="AJ35" s="35"/>
-      <c r="AK35" s="35"/>
-      <c r="AL35" s="35"/>
-      <c r="AM35" s="35"/>
+      <c r="AK35" s="35">
+        <v>7.00</v>
+      </c>
+      <c r="AL35" s="35">
+        <v>7.00</v>
+      </c>
+      <c r="AM35" s="35">
+        <v>7.00</v>
+      </c>
       <c r="AN35" s="35"/>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
@@ -6382,7 +6522,7 @@
       <c r="AJ37" s="10"/>
       <c r="AK37" s="10"/>
       <c r="AL37" s="10"/>
-      <c r="AM37" s="20"/>
+      <c r="AM37" s="20" t="str"/>
       <c r="AN37" s="20"/>
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
@@ -6472,7 +6612,7 @@
       <c r="AJ38" s="23"/>
       <c r="AK38" s="23"/>
       <c r="AL38" s="23"/>
-      <c r="AM38" s="23"/>
+      <c r="AM38" s="23" t="str"/>
       <c r="AN38" s="23"/>
       <c r="AO38" s="23"/>
       <c r="AP38" s="23"/>
@@ -6748,7 +6888,7 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
-      <c r="AM40" s="19"/>
+      <c r="AM40" s="19" t="str"/>
       <c r="AN40" s="19"/>
       <c r="AO40" s="19"/>
       <c r="AP40" s="19"/>
@@ -6864,9 +7004,15 @@
       <c r="AH41" s="10"/>
       <c r="AI41" s="10"/>
       <c r="AJ41" s="10"/>
-      <c r="AK41" s="10"/>
-      <c r="AL41" s="10"/>
-      <c r="AM41" s="20"/>
+      <c r="AK41" s="10">
+        <v>2.50</v>
+      </c>
+      <c r="AL41" s="10">
+        <v>2.50</v>
+      </c>
+      <c r="AM41" s="20">
+        <v>2.50</v>
+      </c>
       <c r="AN41" s="38"/>
       <c r="AO41" s="20"/>
       <c r="AP41" s="20"/>
@@ -6982,9 +7128,15 @@
       <c r="AH42" s="10"/>
       <c r="AI42" s="10"/>
       <c r="AJ42" s="10"/>
-      <c r="AK42" s="10"/>
-      <c r="AL42" s="10"/>
-      <c r="AM42" s="20"/>
+      <c r="AK42" s="10">
+        <v>22.00</v>
+      </c>
+      <c r="AL42" s="10">
+        <v>22.00</v>
+      </c>
+      <c r="AM42" s="20">
+        <v>22.00</v>
+      </c>
       <c r="AN42" s="38"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
@@ -7051,7 +7203,7 @@
       <c r="AJ43" s="10"/>
       <c r="AK43" s="10"/>
       <c r="AL43" s="10"/>
-      <c r="AM43" s="20"/>
+      <c r="AM43" s="20" t="str"/>
       <c r="AN43" s="38"/>
       <c r="AO43" s="20"/>
       <c r="AP43" s="20"/>
@@ -7165,9 +7317,15 @@
       <c r="AH44" s="10"/>
       <c r="AI44" s="10"/>
       <c r="AJ44" s="10"/>
-      <c r="AK44" s="10"/>
-      <c r="AL44" s="10"/>
-      <c r="AM44" s="20"/>
+      <c r="AK44" s="10">
+        <v>24.00</v>
+      </c>
+      <c r="AL44" s="10">
+        <v>24.00</v>
+      </c>
+      <c r="AM44" s="20">
+        <v>24.00</v>
+      </c>
       <c r="AN44" s="38"/>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
@@ -7248,7 +7406,7 @@
       <c r="AJ45" s="10"/>
       <c r="AK45" s="10"/>
       <c r="AL45" s="10"/>
-      <c r="AM45" s="20"/>
+      <c r="AM45" s="20" t="str"/>
       <c r="AN45" s="38"/>
       <c r="AO45" s="20"/>
       <c r="AP45" s="20"/>
@@ -7367,9 +7525,15 @@
       <c r="AH46" s="37"/>
       <c r="AI46" s="37"/>
       <c r="AJ46" s="37"/>
-      <c r="AK46" s="37"/>
-      <c r="AL46" s="37"/>
-      <c r="AM46" s="37"/>
+      <c r="AK46" s="37">
+        <v>12.00</v>
+      </c>
+      <c r="AL46" s="37">
+        <v>12.00</v>
+      </c>
+      <c r="AM46" s="37">
+        <v>12.00</v>
+      </c>
       <c r="AN46" s="37"/>
       <c r="AO46" s="37"/>
       <c r="AP46" s="37"/>
@@ -7645,7 +7809,7 @@
       <c r="AJ48" s="16"/>
       <c r="AK48" s="16"/>
       <c r="AL48" s="16"/>
-      <c r="AM48" s="16"/>
+      <c r="AM48" s="16" t="str"/>
       <c r="AN48" s="16"/>
       <c r="AO48" s="16"/>
       <c r="AP48" s="16"/>
@@ -7918,7 +8082,7 @@
       <c r="AJ50" s="6"/>
       <c r="AK50" s="6"/>
       <c r="AL50" s="6"/>
-      <c r="AM50" s="19"/>
+      <c r="AM50" s="19" t="str"/>
       <c r="AN50" s="19"/>
       <c r="AO50" s="19"/>
       <c r="AP50" s="19"/>
@@ -8030,9 +8194,15 @@
       <c r="AH51" s="10"/>
       <c r="AI51" s="10"/>
       <c r="AJ51" s="10"/>
-      <c r="AK51" s="10"/>
-      <c r="AL51" s="10"/>
-      <c r="AM51" s="20"/>
+      <c r="AK51" s="10">
+        <v>2.25</v>
+      </c>
+      <c r="AL51" s="10">
+        <v>2.25</v>
+      </c>
+      <c r="AM51" s="20">
+        <v>2.25</v>
+      </c>
       <c r="AN51" s="20"/>
       <c r="AO51" s="20"/>
       <c r="AP51" s="20"/>
@@ -8153,7 +8323,9 @@
       <c r="AJ52" s="10"/>
       <c r="AK52" s="10"/>
       <c r="AL52" s="10"/>
-      <c r="AM52" s="20"/>
+      <c r="AM52" s="20">
+        <v>4.75</v>
+      </c>
       <c r="AN52" s="20"/>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
@@ -8260,7 +8432,7 @@
       <c r="AJ53" s="10"/>
       <c r="AK53" s="10"/>
       <c r="AL53" s="10"/>
-      <c r="AM53" s="20"/>
+      <c r="AM53" s="20" t="str"/>
       <c r="AN53" s="20"/>
       <c r="AO53" s="20"/>
       <c r="AP53" s="20"/>
@@ -8536,7 +8708,7 @@
       <c r="AJ55" s="6"/>
       <c r="AK55" s="6"/>
       <c r="AL55" s="6"/>
-      <c r="AM55" s="19"/>
+      <c r="AM55" s="19" t="str"/>
       <c r="BB55" s="6"/>
     </row>
     <row ht="25" r="56" spans="1:54">
@@ -8632,9 +8804,15 @@
       <c r="AH56" s="6"/>
       <c r="AI56" s="6"/>
       <c r="AJ56" s="6"/>
-      <c r="AK56" s="6"/>
-      <c r="AL56" s="6"/>
-      <c r="AM56" s="19"/>
+      <c r="AK56" s="6">
+        <v>8.75</v>
+      </c>
+      <c r="AL56" s="6">
+        <v>8.75</v>
+      </c>
+      <c r="AM56" s="19">
+        <v>8.75</v>
+      </c>
       <c r="AN56" s="37"/>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37"/>
@@ -8730,7 +8908,7 @@
       <c r="AJ57" s="23"/>
       <c r="AK57" s="23"/>
       <c r="AL57" s="23"/>
-      <c r="AM57" s="31"/>
+      <c r="AM57" s="31" t="str"/>
       <c r="AN57" s="35"/>
       <c r="AO57" s="35"/>
       <c r="AP57" s="35"/>
@@ -9002,7 +9180,7 @@
       <c r="AJ59" s="16"/>
       <c r="AK59" s="16"/>
       <c r="AL59" s="16"/>
-      <c r="AM59" s="16"/>
+      <c r="AM59" s="16" t="str"/>
       <c r="AN59" s="16"/>
       <c r="AO59" s="16"/>
       <c r="AP59" s="16"/>
@@ -9105,9 +9283,15 @@
         <v>17</v>
       </c>
       <c r="AJ60" s="37"/>
-      <c r="AK60" s="10"/>
-      <c r="AL60" s="10"/>
-      <c r="AM60" s="106"/>
+      <c r="AK60" s="10">
+        <v>25.00</v>
+      </c>
+      <c r="AL60" s="10">
+        <v>25.00</v>
+      </c>
+      <c r="AM60" s="106">
+        <v>25.00</v>
+      </c>
       <c r="AN60" s="106"/>
       <c r="AO60" s="106"/>
       <c r="AP60" s="106"/>
@@ -9197,9 +9381,15 @@
         <v>29.50</v>
       </c>
       <c r="AJ61" s="37"/>
-      <c r="AK61" s="10"/>
-      <c r="AL61" s="10"/>
-      <c r="AM61" s="106"/>
+      <c r="AK61" s="10">
+        <v>4.00</v>
+      </c>
+      <c r="AL61" s="10">
+        <v>4.00</v>
+      </c>
+      <c r="AM61" s="106">
+        <v>4.00</v>
+      </c>
       <c r="AN61" s="106"/>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
@@ -9288,9 +9478,15 @@
         <v>28.25</v>
       </c>
       <c r="AJ62" s="37"/>
-      <c r="AK62" s="10"/>
-      <c r="AL62" s="10"/>
-      <c r="AM62" s="106"/>
+      <c r="AK62" s="10">
+        <v>16.75</v>
+      </c>
+      <c r="AL62" s="10">
+        <v>16.75</v>
+      </c>
+      <c r="AM62" s="106">
+        <v>16.75</v>
+      </c>
       <c r="AN62" s="106"/>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
@@ -9364,7 +9560,7 @@
       <c r="Y63" s="117"/>
       <c r="Z63" s="117"/>
       <c r="AJ63" s="37"/>
-      <c r="AM63" s="106"/>
+      <c r="AM63" s="106" t="str"/>
       <c r="AN63" s="106"/>
       <c r="AO63" s="106"/>
       <c r="AP63" s="106"/>
@@ -9476,7 +9672,15 @@
         <v>2.50</v>
       </c>
       <c r="AJ64" s="37"/>
-      <c r="AM64" s="106"/>
+      <c r="AK64">
+        <v>2.00</v>
+      </c>
+      <c r="AL64">
+        <v>2.00</v>
+      </c>
+      <c r="AM64" s="106">
+        <v>2.00</v>
+      </c>
       <c r="AN64" s="106"/>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
@@ -9591,7 +9795,15 @@
         <v>13.00</v>
       </c>
       <c r="AJ65" s="37"/>
-      <c r="AM65" s="106"/>
+      <c r="AK65">
+        <v>20.50</v>
+      </c>
+      <c r="AL65">
+        <v>20.50</v>
+      </c>
+      <c r="AM65" s="106">
+        <v>20.50</v>
+      </c>
       <c r="AN65" s="106"/>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
@@ -11302,14 +11514,30 @@
       <c r="AE2" s="1" t="str">
         <v>22.07-28.07.19</v>
       </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="AF2" s="1" t="str">
+        <v>29.07-04.08.19</v>
+      </c>
+      <c r="AG2" s="1" t="str">
+        <v>05.08-11.08.19</v>
+      </c>
+      <c r="AH2" s="1" t="str">
+        <v>12.08-18.08.19</v>
+      </c>
+      <c r="AI2" s="1" t="str">
+        <v>19.08-25.08.19</v>
+      </c>
+      <c r="AJ2" s="1" t="str">
+        <v>26.08-01.09.19</v>
+      </c>
+      <c r="AK2" s="1" t="str">
+        <v>02.09-08.09.19</v>
+      </c>
+      <c r="AL2" s="1" t="str">
+        <v>09.09-15.09.19</v>
+      </c>
+      <c r="AM2" s="1" t="str">
+        <v>16.09-22.09.19</v>
+      </c>
       <c r="AN2" s="18"/>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
@@ -11492,7 +11720,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="AM4" t="str"/>
+    </row>
     <row ht="34" r="5" spans="1:54">
       <c r="A5" s="2" t="s">
         <v>2</v>
@@ -11809,7 +12039,9 @@
       </c>
       <c r="BB6" s="3"/>
     </row>
-    <row r="7"/>
+    <row r="7">
+      <c r="AM7" t="str"/>
+    </row>
     <row ht="25" r="8" spans="1:54">
       <c r="A8" s="5" t="s">
         <v>104</v>
@@ -11907,7 +12139,7 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="19"/>
+      <c r="AM8" s="19" t="str"/>
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
@@ -12014,7 +12246,7 @@
       <c r="AJ9" s="6"/>
       <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="19"/>
+      <c r="AM9" s="19" t="str"/>
       <c r="AN9" s="19"/>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
@@ -12290,7 +12522,7 @@
       <c r="AJ11" s="6"/>
       <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="19"/>
+      <c r="AM11" s="19" t="str"/>
       <c r="AN11" s="19"/>
       <c r="AO11" s="19"/>
       <c r="AP11" s="19"/>
@@ -12394,7 +12626,7 @@
       <c r="AJ12" s="10"/>
       <c r="AK12" s="10"/>
       <c r="AL12" s="10"/>
-      <c r="AM12" s="20"/>
+      <c r="AM12" s="20" t="str"/>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20"/>
@@ -12471,7 +12703,7 @@
       <c r="AJ13" s="10"/>
       <c r="AK13" s="10"/>
       <c r="AL13" s="10"/>
-      <c r="AM13" s="20"/>
+      <c r="AM13" s="20" t="str"/>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
@@ -12579,7 +12811,7 @@
       <c r="AJ14" s="10"/>
       <c r="AK14" s="10"/>
       <c r="AL14" s="10"/>
-      <c r="AM14" s="20"/>
+      <c r="AM14" s="20" t="str"/>
       <c r="AN14" s="38"/>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
@@ -12686,7 +12918,7 @@
       <c r="AJ15" s="10"/>
       <c r="AK15" s="10"/>
       <c r="AL15" s="10"/>
-      <c r="AM15" s="20"/>
+      <c r="AM15" s="20" t="str"/>
       <c r="AN15" s="38"/>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
@@ -12793,7 +13025,7 @@
       <c r="AJ16" s="10"/>
       <c r="AK16" s="10"/>
       <c r="AL16" s="10"/>
-      <c r="AM16" s="20"/>
+      <c r="AM16" s="20" t="str"/>
       <c r="AN16" s="38"/>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
@@ -12900,7 +13132,7 @@
       <c r="AJ17" s="10"/>
       <c r="AK17" s="10"/>
       <c r="AL17" s="10"/>
-      <c r="AM17" s="20"/>
+      <c r="AM17" s="20" t="str"/>
       <c r="AN17" s="38"/>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20"/>
@@ -12997,7 +13229,7 @@
       <c r="AJ18" s="10"/>
       <c r="AK18" s="10"/>
       <c r="AL18" s="10"/>
-      <c r="AM18" s="20"/>
+      <c r="AM18" s="20" t="str"/>
       <c r="AN18" s="38"/>
       <c r="AO18" s="20"/>
       <c r="AP18" s="20"/>
@@ -13104,7 +13336,7 @@
       <c r="AJ19" s="10"/>
       <c r="AK19" s="10"/>
       <c r="AL19" s="10"/>
-      <c r="AM19" s="20"/>
+      <c r="AM19" s="20" t="str"/>
       <c r="AN19" s="38"/>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
@@ -13215,7 +13447,7 @@
       <c r="AJ20" s="10"/>
       <c r="AK20" s="10"/>
       <c r="AL20" s="10"/>
-      <c r="AM20" s="37"/>
+      <c r="AM20" s="37" t="str"/>
       <c r="AN20" s="37"/>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
@@ -13322,7 +13554,7 @@
       <c r="AJ21" s="35"/>
       <c r="AK21" s="35"/>
       <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
+      <c r="AM21" s="35" t="str"/>
       <c r="AN21" s="35"/>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
@@ -13431,7 +13663,7 @@
       <c r="AJ22" s="35"/>
       <c r="AK22" s="35"/>
       <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
+      <c r="AM22" s="35" t="str"/>
       <c r="AN22" s="35"/>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
@@ -13707,7 +13939,7 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
-      <c r="AM24" s="19"/>
+      <c r="AM24" s="19" t="str"/>
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
       <c r="AP24" s="19"/>
@@ -13811,7 +14043,7 @@
       <c r="AJ25" s="6"/>
       <c r="AK25" s="6"/>
       <c r="AL25" s="6"/>
-      <c r="AM25" s="19"/>
+      <c r="AM25" s="19" t="str"/>
       <c r="AN25" s="19"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
@@ -13917,7 +14149,7 @@
       <c r="AJ26" s="10"/>
       <c r="AK26" s="10"/>
       <c r="AL26" s="10"/>
-      <c r="AM26" s="20"/>
+      <c r="AM26" s="20" t="str"/>
       <c r="AN26" s="38"/>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
@@ -14024,7 +14256,7 @@
       <c r="AJ27" s="10"/>
       <c r="AK27" s="10"/>
       <c r="AL27" s="10"/>
-      <c r="AM27" s="20"/>
+      <c r="AM27" s="20" t="str"/>
       <c r="AN27" s="38"/>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
@@ -14131,7 +14363,7 @@
       <c r="AJ28" s="10"/>
       <c r="AK28" s="10"/>
       <c r="AL28" s="10"/>
-      <c r="AM28" s="20"/>
+      <c r="AM28" s="20" t="str"/>
       <c r="AN28" s="38"/>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
@@ -14235,7 +14467,7 @@
       <c r="AJ29" s="10"/>
       <c r="AK29" s="10"/>
       <c r="AL29" s="10"/>
-      <c r="AM29" s="20"/>
+      <c r="AM29" s="20" t="str"/>
       <c r="AN29" s="38"/>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
@@ -14339,7 +14571,7 @@
       <c r="AJ30" s="10"/>
       <c r="AK30" s="10"/>
       <c r="AL30" s="10"/>
-      <c r="AM30" s="20"/>
+      <c r="AM30" s="20" t="str"/>
       <c r="AN30" s="38"/>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
@@ -14446,7 +14678,7 @@
       <c r="AJ31" s="10"/>
       <c r="AK31" s="10"/>
       <c r="AL31" s="10"/>
-      <c r="AM31" s="20"/>
+      <c r="AM31" s="20" t="str"/>
       <c r="AN31" s="38"/>
       <c r="AO31" s="20"/>
       <c r="AP31" s="20"/>
@@ -14553,7 +14785,7 @@
       <c r="AJ32" s="10"/>
       <c r="AK32" s="10"/>
       <c r="AL32" s="10"/>
-      <c r="AM32" s="20"/>
+      <c r="AM32" s="20" t="str"/>
       <c r="AN32" s="38"/>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
@@ -14660,7 +14892,7 @@
       <c r="AJ33" s="10"/>
       <c r="AK33" s="10"/>
       <c r="AL33" s="10"/>
-      <c r="AM33" s="20"/>
+      <c r="AM33" s="20" t="str"/>
       <c r="AN33" s="38"/>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
@@ -14767,7 +14999,7 @@
       <c r="AJ34" s="35"/>
       <c r="AK34" s="35"/>
       <c r="AL34" s="35"/>
-      <c r="AM34" s="35"/>
+      <c r="AM34" s="35" t="str"/>
       <c r="AN34" s="35"/>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
@@ -14874,7 +15106,7 @@
       <c r="AJ35" s="35"/>
       <c r="AK35" s="35"/>
       <c r="AL35" s="35"/>
-      <c r="AM35" s="35"/>
+      <c r="AM35" s="35" t="str"/>
       <c r="AN35" s="35"/>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
@@ -15150,7 +15382,7 @@
       <c r="AJ37" s="10"/>
       <c r="AK37" s="10"/>
       <c r="AL37" s="10"/>
-      <c r="AM37" s="20"/>
+      <c r="AM37" s="20" t="str"/>
       <c r="AN37" s="20"/>
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
@@ -15240,7 +15472,7 @@
       <c r="AJ38" s="23"/>
       <c r="AK38" s="23"/>
       <c r="AL38" s="23"/>
-      <c r="AM38" s="23"/>
+      <c r="AM38" s="23" t="str"/>
       <c r="AN38" s="23"/>
       <c r="AO38" s="23"/>
       <c r="AP38" s="23"/>
@@ -15516,7 +15748,7 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
-      <c r="AM40" s="19"/>
+      <c r="AM40" s="19" t="str"/>
       <c r="AN40" s="19"/>
       <c r="AO40" s="19"/>
       <c r="AP40" s="19"/>
@@ -15620,7 +15852,7 @@
       <c r="AJ41" s="10"/>
       <c r="AK41" s="10"/>
       <c r="AL41" s="10"/>
-      <c r="AM41" s="20"/>
+      <c r="AM41" s="20" t="str"/>
       <c r="AN41" s="38"/>
       <c r="AO41" s="20"/>
       <c r="AP41" s="20"/>
@@ -15727,7 +15959,7 @@
       <c r="AJ42" s="10"/>
       <c r="AK42" s="10"/>
       <c r="AL42" s="10"/>
-      <c r="AM42" s="20"/>
+      <c r="AM42" s="20" t="str"/>
       <c r="AN42" s="38"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
@@ -15788,7 +16020,7 @@
       <c r="AJ43" s="10"/>
       <c r="AK43" s="10"/>
       <c r="AL43" s="10"/>
-      <c r="AM43" s="20"/>
+      <c r="AM43" s="20" t="str"/>
       <c r="AN43" s="38"/>
       <c r="AO43" s="20"/>
       <c r="AP43" s="20"/>
@@ -15892,7 +16124,7 @@
       <c r="AJ44" s="10"/>
       <c r="AK44" s="10"/>
       <c r="AL44" s="10"/>
-      <c r="AM44" s="20"/>
+      <c r="AM44" s="20" t="str"/>
       <c r="AN44" s="38"/>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
@@ -15971,7 +16203,7 @@
       <c r="AJ45" s="10"/>
       <c r="AK45" s="10"/>
       <c r="AL45" s="10"/>
-      <c r="AM45" s="20"/>
+      <c r="AM45" s="20" t="str"/>
       <c r="AN45" s="38"/>
       <c r="AO45" s="20"/>
       <c r="AP45" s="20"/>
@@ -16079,7 +16311,7 @@
       <c r="AJ46" s="37"/>
       <c r="AK46" s="37"/>
       <c r="AL46" s="37"/>
-      <c r="AM46" s="37"/>
+      <c r="AM46" s="37" t="str"/>
       <c r="AN46" s="37"/>
       <c r="AO46" s="37"/>
       <c r="AP46" s="37"/>
@@ -16355,7 +16587,7 @@
       <c r="AJ48" s="16"/>
       <c r="AK48" s="16"/>
       <c r="AL48" s="16"/>
-      <c r="AM48" s="16"/>
+      <c r="AM48" s="16" t="str"/>
       <c r="AN48" s="16"/>
       <c r="AO48" s="16"/>
       <c r="AP48" s="16"/>
@@ -16628,7 +16860,7 @@
       <c r="AJ50" s="6"/>
       <c r="AK50" s="6"/>
       <c r="AL50" s="6"/>
-      <c r="AM50" s="19"/>
+      <c r="AM50" s="19" t="str"/>
       <c r="AN50" s="19"/>
       <c r="AO50" s="19"/>
       <c r="AP50" s="19"/>
@@ -16732,7 +16964,7 @@
       <c r="AJ51" s="10"/>
       <c r="AK51" s="10"/>
       <c r="AL51" s="10"/>
-      <c r="AM51" s="20"/>
+      <c r="AM51" s="20" t="str"/>
       <c r="AN51" s="20"/>
       <c r="AO51" s="20"/>
       <c r="AP51" s="20"/>
@@ -16839,7 +17071,7 @@
       <c r="AJ52" s="10"/>
       <c r="AK52" s="10"/>
       <c r="AL52" s="10"/>
-      <c r="AM52" s="20"/>
+      <c r="AM52" s="20" t="str"/>
       <c r="AN52" s="20"/>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
@@ -16946,7 +17178,7 @@
       <c r="AJ53" s="10"/>
       <c r="AK53" s="10"/>
       <c r="AL53" s="10"/>
-      <c r="AM53" s="20"/>
+      <c r="AM53" s="20" t="str"/>
       <c r="AN53" s="20"/>
       <c r="AO53" s="20"/>
       <c r="AP53" s="20"/>
@@ -17222,7 +17454,7 @@
       <c r="AJ55" s="6"/>
       <c r="AK55" s="6"/>
       <c r="AL55" s="6"/>
-      <c r="AM55" s="19"/>
+      <c r="AM55" s="19" t="str"/>
       <c r="BB55" s="6"/>
     </row>
     <row ht="25" r="56" spans="1:54">
@@ -17312,7 +17544,7 @@
       <c r="AJ56" s="6"/>
       <c r="AK56" s="6"/>
       <c r="AL56" s="6"/>
-      <c r="AM56" s="19"/>
+      <c r="AM56" s="19" t="str"/>
       <c r="AN56" s="37"/>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37"/>
@@ -17404,7 +17636,7 @@
       <c r="AJ57" s="23"/>
       <c r="AK57" s="23"/>
       <c r="AL57" s="23"/>
-      <c r="AM57" s="31"/>
+      <c r="AM57" s="31" t="str"/>
       <c r="AN57" s="35"/>
       <c r="AO57" s="35"/>
       <c r="AP57" s="35"/>
@@ -17676,7 +17908,7 @@
       <c r="AJ59" s="16"/>
       <c r="AK59" s="16"/>
       <c r="AL59" s="16"/>
-      <c r="AM59" s="16"/>
+      <c r="AM59" s="16" t="str"/>
       <c r="AN59" s="16"/>
       <c r="AO59" s="16"/>
       <c r="AP59" s="16"/>
@@ -17769,7 +18001,7 @@
       <c r="AJ60" s="37"/>
       <c r="AK60" s="10"/>
       <c r="AL60" s="10"/>
-      <c r="AM60" s="106"/>
+      <c r="AM60" s="106" t="str"/>
       <c r="AN60" s="106"/>
       <c r="AO60" s="106"/>
       <c r="AP60" s="106"/>
@@ -17843,7 +18075,7 @@
       <c r="AJ61" s="37"/>
       <c r="AK61" s="10"/>
       <c r="AL61" s="10"/>
-      <c r="AM61" s="106"/>
+      <c r="AM61" s="106" t="str"/>
       <c r="AN61" s="106"/>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
@@ -17910,7 +18142,7 @@
       <c r="AJ62" s="37"/>
       <c r="AK62" s="10"/>
       <c r="AL62" s="10"/>
-      <c r="AM62" s="106"/>
+      <c r="AM62" s="106" t="str"/>
       <c r="AN62" s="106"/>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
@@ -17981,7 +18213,7 @@
       <c r="Y63" s="117"/>
       <c r="Z63" s="117"/>
       <c r="AJ63" s="37"/>
-      <c r="AM63" s="106"/>
+      <c r="AM63" s="106" t="str"/>
       <c r="AN63" s="106"/>
       <c r="AO63" s="106"/>
       <c r="AP63" s="106"/>
@@ -18075,7 +18307,7 @@
         <v>0</v>
       </c>
       <c r="AJ64" s="37"/>
-      <c r="AM64" s="106"/>
+      <c r="AM64" s="106" t="str"/>
       <c r="AN64" s="106"/>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
@@ -18169,7 +18401,7 @@
         <v>0</v>
       </c>
       <c r="AJ65" s="37"/>
-      <c r="AM65" s="106"/>
+      <c r="AM65" s="106" t="str"/>
       <c r="AN65" s="106"/>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
@@ -18801,14 +19033,30 @@
       <c r="AE2" s="1" t="str">
         <v>22.07-28.07.19</v>
       </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="AF2" s="1" t="str">
+        <v>29.07-04.08.19</v>
+      </c>
+      <c r="AG2" s="1" t="str">
+        <v>05.08-11.08.19</v>
+      </c>
+      <c r="AH2" s="1" t="str">
+        <v>12.08-18.08.19</v>
+      </c>
+      <c r="AI2" s="1" t="str">
+        <v>19.08-25.08.19</v>
+      </c>
+      <c r="AJ2" s="1" t="str">
+        <v>26.08-01.09.19</v>
+      </c>
+      <c r="AK2" s="1" t="str">
+        <v>02.09-08.09.19</v>
+      </c>
+      <c r="AL2" s="1" t="str">
+        <v>09.09-15.09.19</v>
+      </c>
+      <c r="AM2" s="1" t="str">
+        <v>16.09-22.09.19</v>
+      </c>
       <c r="AN2" s="18"/>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
@@ -18995,6 +19243,7 @@
       <c r="J4" t="s">
         <v>90</v>
       </c>
+      <c r="AM4" t="str"/>
     </row>
     <row ht="34" r="5" spans="1:54">
       <c r="A5" s="2" t="s">
@@ -19312,7 +19561,9 @@
       </c>
       <c r="BB6" s="3"/>
     </row>
-    <row r="7"/>
+    <row r="7">
+      <c r="AM7" t="str"/>
+    </row>
     <row ht="25" r="8" spans="1:54">
       <c r="A8" s="5" t="s">
         <v>104</v>
@@ -19400,7 +19651,7 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="19"/>
+      <c r="AM8" s="19" t="str"/>
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
@@ -19507,7 +19758,7 @@
       <c r="AJ9" s="6"/>
       <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="19"/>
+      <c r="AM9" s="19" t="str"/>
       <c r="AN9" s="19"/>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
@@ -19783,7 +20034,7 @@
       <c r="AJ11" s="6"/>
       <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="19"/>
+      <c r="AM11" s="19" t="str"/>
       <c r="AN11" s="19"/>
       <c r="AO11" s="19"/>
       <c r="AP11" s="19"/>
@@ -19893,7 +20144,7 @@
       <c r="AJ12" s="10"/>
       <c r="AK12" s="10"/>
       <c r="AL12" s="10"/>
-      <c r="AM12" s="20"/>
+      <c r="AM12" s="20" t="str"/>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20"/>
@@ -19966,7 +20217,7 @@
       <c r="AJ13" s="10"/>
       <c r="AK13" s="10"/>
       <c r="AL13" s="10"/>
-      <c r="AM13" s="20"/>
+      <c r="AM13" s="20" t="str"/>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
@@ -20080,9 +20331,15 @@
       <c r="AH14" s="10"/>
       <c r="AI14" s="10"/>
       <c r="AJ14" s="10"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="10"/>
-      <c r="AM14" s="20"/>
+      <c r="AK14" s="10">
+        <v>3.00</v>
+      </c>
+      <c r="AL14" s="10">
+        <v>3.00</v>
+      </c>
+      <c r="AM14" s="20">
+        <v>3.00</v>
+      </c>
       <c r="AN14" s="38"/>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
@@ -20193,9 +20450,15 @@
       <c r="AH15" s="10"/>
       <c r="AI15" s="10"/>
       <c r="AJ15" s="10"/>
-      <c r="AK15" s="10"/>
-      <c r="AL15" s="10"/>
-      <c r="AM15" s="20"/>
+      <c r="AK15" s="10">
+        <v>5.00</v>
+      </c>
+      <c r="AL15" s="10">
+        <v>5.00</v>
+      </c>
+      <c r="AM15" s="20">
+        <v>5.00</v>
+      </c>
       <c r="AN15" s="38"/>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
@@ -20311,7 +20574,9 @@
       <c r="AJ16" s="10"/>
       <c r="AK16" s="10"/>
       <c r="AL16" s="10"/>
-      <c r="AM16" s="20"/>
+      <c r="AM16" s="20">
+        <v>5.50</v>
+      </c>
       <c r="AN16" s="38"/>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
@@ -20418,7 +20683,7 @@
       <c r="AJ17" s="10"/>
       <c r="AK17" s="10"/>
       <c r="AL17" s="10"/>
-      <c r="AM17" s="20"/>
+      <c r="AM17" s="20" t="str"/>
       <c r="AN17" s="38"/>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20"/>
@@ -20515,7 +20780,7 @@
       <c r="AJ18" s="10"/>
       <c r="AK18" s="10"/>
       <c r="AL18" s="10"/>
-      <c r="AM18" s="20"/>
+      <c r="AM18" s="20" t="str"/>
       <c r="AN18" s="38"/>
       <c r="AO18" s="20"/>
       <c r="AP18" s="20"/>
@@ -20634,9 +20899,15 @@
       <c r="AH19" s="10"/>
       <c r="AI19" s="10"/>
       <c r="AJ19" s="10"/>
-      <c r="AK19" s="10"/>
-      <c r="AL19" s="10"/>
-      <c r="AM19" s="20"/>
+      <c r="AK19" s="10">
+        <v>4.00</v>
+      </c>
+      <c r="AL19" s="10">
+        <v>4.00</v>
+      </c>
+      <c r="AM19" s="20">
+        <v>4.00</v>
+      </c>
       <c r="AN19" s="38"/>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
@@ -20751,9 +21022,15 @@
       <c r="AH20" s="10"/>
       <c r="AI20" s="10"/>
       <c r="AJ20" s="10"/>
-      <c r="AK20" s="10"/>
-      <c r="AL20" s="10"/>
-      <c r="AM20" s="37"/>
+      <c r="AK20" s="10">
+        <v>7.25</v>
+      </c>
+      <c r="AL20" s="10">
+        <v>7.25</v>
+      </c>
+      <c r="AM20" s="37">
+        <v>7.25</v>
+      </c>
       <c r="AN20" s="37"/>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
@@ -20860,7 +21137,7 @@
       <c r="AJ21" s="35"/>
       <c r="AK21" s="35"/>
       <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
+      <c r="AM21" s="35" t="str"/>
       <c r="AN21" s="35"/>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
@@ -20977,9 +21254,15 @@
       <c r="AH22" s="35"/>
       <c r="AI22" s="35"/>
       <c r="AJ22" s="35"/>
-      <c r="AK22" s="35"/>
-      <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
+      <c r="AK22" s="35">
+        <v>15.00</v>
+      </c>
+      <c r="AL22" s="35">
+        <v>15.00</v>
+      </c>
+      <c r="AM22" s="35">
+        <v>15.00</v>
+      </c>
       <c r="AN22" s="35"/>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
@@ -21255,7 +21538,7 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
-      <c r="AM24" s="19"/>
+      <c r="AM24" s="19" t="str"/>
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
       <c r="AP24" s="19"/>
@@ -21369,7 +21652,7 @@
       <c r="AJ25" s="6"/>
       <c r="AK25" s="6"/>
       <c r="AL25" s="6"/>
-      <c r="AM25" s="19"/>
+      <c r="AM25" s="19" t="str"/>
       <c r="AN25" s="19"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
@@ -21473,7 +21756,7 @@
       <c r="AJ26" s="10"/>
       <c r="AK26" s="10"/>
       <c r="AL26" s="10"/>
-      <c r="AM26" s="20"/>
+      <c r="AM26" s="20" t="str"/>
       <c r="AN26" s="38"/>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
@@ -21592,9 +21875,15 @@
       <c r="AH27" s="10"/>
       <c r="AI27" s="10"/>
       <c r="AJ27" s="10"/>
-      <c r="AK27" s="10"/>
-      <c r="AL27" s="10"/>
-      <c r="AM27" s="20"/>
+      <c r="AK27" s="10">
+        <v>2.75</v>
+      </c>
+      <c r="AL27" s="10">
+        <v>2.75</v>
+      </c>
+      <c r="AM27" s="20">
+        <v>2.75</v>
+      </c>
       <c r="AN27" s="38"/>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
@@ -21701,7 +21990,7 @@
       <c r="AJ28" s="10"/>
       <c r="AK28" s="10"/>
       <c r="AL28" s="10"/>
-      <c r="AM28" s="20"/>
+      <c r="AM28" s="20" t="str"/>
       <c r="AN28" s="38"/>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
@@ -21811,7 +22100,7 @@
       <c r="AJ29" s="10"/>
       <c r="AK29" s="10"/>
       <c r="AL29" s="10"/>
-      <c r="AM29" s="20"/>
+      <c r="AM29" s="20" t="str"/>
       <c r="AN29" s="38"/>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
@@ -21925,9 +22214,15 @@
       <c r="AH30" s="10"/>
       <c r="AI30" s="10"/>
       <c r="AJ30" s="10"/>
-      <c r="AK30" s="10"/>
-      <c r="AL30" s="10"/>
-      <c r="AM30" s="20"/>
+      <c r="AK30" s="10">
+        <v>0.50</v>
+      </c>
+      <c r="AL30" s="10">
+        <v>0.50</v>
+      </c>
+      <c r="AM30" s="20">
+        <v>0.50</v>
+      </c>
       <c r="AN30" s="38"/>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
@@ -22042,7 +22337,7 @@
       <c r="AJ31" s="10"/>
       <c r="AK31" s="10"/>
       <c r="AL31" s="10"/>
-      <c r="AM31" s="20"/>
+      <c r="AM31" s="20" t="str"/>
       <c r="AN31" s="38"/>
       <c r="AO31" s="20"/>
       <c r="AP31" s="20"/>
@@ -22159,9 +22454,15 @@
       <c r="AH32" s="10"/>
       <c r="AI32" s="10"/>
       <c r="AJ32" s="10"/>
-      <c r="AK32" s="10"/>
-      <c r="AL32" s="10"/>
-      <c r="AM32" s="20"/>
+      <c r="AK32" s="10">
+        <v>6.50</v>
+      </c>
+      <c r="AL32" s="10">
+        <v>6.50</v>
+      </c>
+      <c r="AM32" s="20">
+        <v>6.50</v>
+      </c>
       <c r="AN32" s="38"/>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
@@ -22280,9 +22581,15 @@
       <c r="AH33" s="10"/>
       <c r="AI33" s="10"/>
       <c r="AJ33" s="10"/>
-      <c r="AK33" s="10"/>
-      <c r="AL33" s="10"/>
-      <c r="AM33" s="20"/>
+      <c r="AK33" s="10">
+        <v>2.25</v>
+      </c>
+      <c r="AL33" s="10">
+        <v>2.25</v>
+      </c>
+      <c r="AM33" s="20">
+        <v>2.25</v>
+      </c>
       <c r="AN33" s="38"/>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
@@ -22393,7 +22700,7 @@
       <c r="AJ34" s="35"/>
       <c r="AK34" s="35"/>
       <c r="AL34" s="35"/>
-      <c r="AM34" s="35"/>
+      <c r="AM34" s="35" t="str"/>
       <c r="AN34" s="35"/>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
@@ -22500,7 +22807,7 @@
       <c r="AJ35" s="35"/>
       <c r="AK35" s="35"/>
       <c r="AL35" s="35"/>
-      <c r="AM35" s="35"/>
+      <c r="AM35" s="35" t="str"/>
       <c r="AN35" s="35"/>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
@@ -22776,7 +23083,7 @@
       <c r="AJ37" s="10"/>
       <c r="AK37" s="10"/>
       <c r="AL37" s="10"/>
-      <c r="AM37" s="20"/>
+      <c r="AM37" s="20" t="str"/>
       <c r="AN37" s="20"/>
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
@@ -22866,7 +23173,7 @@
       <c r="AJ38" s="23"/>
       <c r="AK38" s="23"/>
       <c r="AL38" s="23"/>
-      <c r="AM38" s="23"/>
+      <c r="AM38" s="23" t="str"/>
       <c r="AN38" s="23"/>
       <c r="AO38" s="23"/>
       <c r="AP38" s="23"/>
@@ -23142,7 +23449,7 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
-      <c r="AM40" s="19"/>
+      <c r="AM40" s="19" t="str"/>
       <c r="AN40" s="19"/>
       <c r="AO40" s="19"/>
       <c r="AP40" s="19"/>
@@ -23246,7 +23553,7 @@
       <c r="AJ41" s="10"/>
       <c r="AK41" s="10"/>
       <c r="AL41" s="10"/>
-      <c r="AM41" s="20"/>
+      <c r="AM41" s="20" t="str"/>
       <c r="AN41" s="38"/>
       <c r="AO41" s="20"/>
       <c r="AP41" s="20"/>
@@ -23359,9 +23666,15 @@
       <c r="AH42" s="10"/>
       <c r="AI42" s="10"/>
       <c r="AJ42" s="10"/>
-      <c r="AK42" s="10"/>
-      <c r="AL42" s="10"/>
-      <c r="AM42" s="20"/>
+      <c r="AK42" s="10">
+        <v>7.00</v>
+      </c>
+      <c r="AL42" s="10">
+        <v>7.00</v>
+      </c>
+      <c r="AM42" s="20">
+        <v>7.00</v>
+      </c>
       <c r="AN42" s="38"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
@@ -23422,7 +23735,7 @@
       <c r="AJ43" s="10"/>
       <c r="AK43" s="10"/>
       <c r="AL43" s="10"/>
-      <c r="AM43" s="20"/>
+      <c r="AM43" s="20" t="str"/>
       <c r="AN43" s="38"/>
       <c r="AO43" s="20"/>
       <c r="AP43" s="20"/>
@@ -23536,9 +23849,15 @@
       <c r="AH44" s="10"/>
       <c r="AI44" s="10"/>
       <c r="AJ44" s="10"/>
-      <c r="AK44" s="10"/>
-      <c r="AL44" s="10"/>
-      <c r="AM44" s="20"/>
+      <c r="AK44" s="10">
+        <v>3.50</v>
+      </c>
+      <c r="AL44" s="10">
+        <v>3.50</v>
+      </c>
+      <c r="AM44" s="20">
+        <v>3.50</v>
+      </c>
       <c r="AN44" s="38"/>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
@@ -23617,7 +23936,7 @@
       <c r="AJ45" s="10"/>
       <c r="AK45" s="10"/>
       <c r="AL45" s="10"/>
-      <c r="AM45" s="20"/>
+      <c r="AM45" s="20" t="str"/>
       <c r="AN45" s="38"/>
       <c r="AO45" s="20"/>
       <c r="AP45" s="20"/>
@@ -23721,7 +24040,7 @@
       <c r="AJ46" s="37"/>
       <c r="AK46" s="37"/>
       <c r="AL46" s="37"/>
-      <c r="AM46" s="37"/>
+      <c r="AM46" s="37" t="str"/>
       <c r="AN46" s="37"/>
       <c r="AO46" s="37"/>
       <c r="AP46" s="37"/>
@@ -23997,7 +24316,7 @@
       <c r="AJ48" s="16"/>
       <c r="AK48" s="16"/>
       <c r="AL48" s="16"/>
-      <c r="AM48" s="16"/>
+      <c r="AM48" s="16" t="str"/>
       <c r="AN48" s="16"/>
       <c r="AO48" s="16"/>
       <c r="AP48" s="16"/>
@@ -24270,7 +24589,7 @@
       <c r="AJ50" s="6"/>
       <c r="AK50" s="6"/>
       <c r="AL50" s="6"/>
-      <c r="AM50" s="19"/>
+      <c r="AM50" s="19" t="str"/>
       <c r="AN50" s="19"/>
       <c r="AO50" s="19"/>
       <c r="AP50" s="19"/>
@@ -24374,7 +24693,7 @@
       <c r="AJ51" s="10"/>
       <c r="AK51" s="10"/>
       <c r="AL51" s="10"/>
-      <c r="AM51" s="20"/>
+      <c r="AM51" s="20" t="str"/>
       <c r="AN51" s="20"/>
       <c r="AO51" s="20"/>
       <c r="AP51" s="20"/>
@@ -24493,7 +24812,9 @@
       <c r="AJ52" s="10"/>
       <c r="AK52" s="10"/>
       <c r="AL52" s="10"/>
-      <c r="AM52" s="20"/>
+      <c r="AM52" s="20">
+        <v>2.25</v>
+      </c>
       <c r="AN52" s="20"/>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
@@ -24600,7 +24921,7 @@
       <c r="AJ53" s="10"/>
       <c r="AK53" s="10"/>
       <c r="AL53" s="10"/>
-      <c r="AM53" s="20"/>
+      <c r="AM53" s="20" t="str"/>
       <c r="AN53" s="20"/>
       <c r="AO53" s="20"/>
       <c r="AP53" s="20"/>
@@ -24876,7 +25197,7 @@
       <c r="AJ55" s="6"/>
       <c r="AK55" s="6"/>
       <c r="AL55" s="6"/>
-      <c r="AM55" s="19"/>
+      <c r="AM55" s="19" t="str"/>
       <c r="BB55" s="6"/>
     </row>
     <row ht="25" r="56" spans="1:54">
@@ -24966,7 +25287,7 @@
       <c r="AJ56" s="6"/>
       <c r="AK56" s="6"/>
       <c r="AL56" s="6"/>
-      <c r="AM56" s="19"/>
+      <c r="AM56" s="19" t="str"/>
       <c r="AN56" s="37"/>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37"/>
@@ -25058,7 +25379,7 @@
       <c r="AJ57" s="23"/>
       <c r="AK57" s="23"/>
       <c r="AL57" s="23"/>
-      <c r="AM57" s="31"/>
+      <c r="AM57" s="31" t="str"/>
       <c r="AN57" s="35"/>
       <c r="AO57" s="35"/>
       <c r="AP57" s="35"/>
@@ -25330,7 +25651,7 @@
       <c r="AJ59" s="16"/>
       <c r="AK59" s="16"/>
       <c r="AL59" s="16"/>
-      <c r="AM59" s="16"/>
+      <c r="AM59" s="16" t="str"/>
       <c r="AN59" s="16"/>
       <c r="AO59" s="16"/>
       <c r="AP59" s="16"/>
@@ -25423,7 +25744,7 @@
       <c r="AJ60" s="37"/>
       <c r="AK60" s="10"/>
       <c r="AL60" s="10"/>
-      <c r="AM60" s="106"/>
+      <c r="AM60" s="106" t="str"/>
       <c r="AN60" s="106"/>
       <c r="AO60" s="106"/>
       <c r="AP60" s="106"/>
@@ -25497,7 +25818,7 @@
       <c r="AJ61" s="37"/>
       <c r="AK61" s="10"/>
       <c r="AL61" s="10"/>
-      <c r="AM61" s="106"/>
+      <c r="AM61" s="106" t="str"/>
       <c r="AN61" s="106"/>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
@@ -25568,9 +25889,15 @@
         <v>0.5</v>
       </c>
       <c r="AJ62" s="37"/>
-      <c r="AK62" s="10"/>
-      <c r="AL62" s="10"/>
-      <c r="AM62" s="106"/>
+      <c r="AK62" s="10">
+        <v>0.50</v>
+      </c>
+      <c r="AL62" s="10">
+        <v>0.50</v>
+      </c>
+      <c r="AM62" s="106">
+        <v>0.50</v>
+      </c>
       <c r="AN62" s="106"/>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
@@ -25641,7 +25968,7 @@
       <c r="Y63" s="117"/>
       <c r="Z63" s="117"/>
       <c r="AJ63" s="37"/>
-      <c r="AM63" s="106"/>
+      <c r="AM63" s="106" t="str"/>
       <c r="AN63" s="106"/>
       <c r="AO63" s="106"/>
       <c r="AP63" s="106"/>
@@ -25741,7 +26068,15 @@
         <v>4</v>
       </c>
       <c r="AJ64" s="37"/>
-      <c r="AM64" s="106"/>
+      <c r="AK64">
+        <v>1.50</v>
+      </c>
+      <c r="AL64">
+        <v>1.50</v>
+      </c>
+      <c r="AM64" s="106">
+        <v>1.50</v>
+      </c>
       <c r="AN64" s="106"/>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
@@ -25838,7 +26173,15 @@
         <v>3</v>
       </c>
       <c r="AJ65" s="37"/>
-      <c r="AM65" s="106"/>
+      <c r="AK65">
+        <v>4.00</v>
+      </c>
+      <c r="AL65">
+        <v>4.00</v>
+      </c>
+      <c r="AM65" s="106">
+        <v>4.00</v>
+      </c>
       <c r="AN65" s="106"/>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
@@ -26471,14 +26814,30 @@
       <c r="AE2" s="1" t="str">
         <v>22.07-28.07.19</v>
       </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="AF2" s="1" t="str">
+        <v>29.07-04.08.19</v>
+      </c>
+      <c r="AG2" s="1" t="str">
+        <v>05.08-11.08.19</v>
+      </c>
+      <c r="AH2" s="1" t="str">
+        <v>12.08-18.08.19</v>
+      </c>
+      <c r="AI2" s="1" t="str">
+        <v>19.08-25.08.19</v>
+      </c>
+      <c r="AJ2" s="1" t="str">
+        <v>26.08-01.09.19</v>
+      </c>
+      <c r="AK2" s="1" t="str">
+        <v>02.09-08.09.19</v>
+      </c>
+      <c r="AL2" s="1" t="str">
+        <v>09.09-15.09.19</v>
+      </c>
+      <c r="AM2" s="1" t="str">
+        <v>16.09-22.09.19</v>
+      </c>
       <c r="AN2" s="18"/>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
@@ -26661,7 +27020,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="AM4" t="str"/>
+    </row>
     <row ht="34" r="5" spans="1:54">
       <c r="A5" s="2" t="s">
         <v>2</v>
@@ -26978,7 +27339,9 @@
       </c>
       <c r="BB6" s="3"/>
     </row>
-    <row r="7"/>
+    <row r="7">
+      <c r="AM7" t="str"/>
+    </row>
     <row ht="25" r="8" spans="1:54">
       <c r="A8" s="5" t="s">
         <v>104</v>
@@ -27078,9 +27441,15 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="6"/>
       <c r="AJ8" s="6"/>
-      <c r="AK8" s="6"/>
-      <c r="AL8" s="6"/>
-      <c r="AM8" s="19"/>
+      <c r="AK8" s="6">
+        <v>4.75</v>
+      </c>
+      <c r="AL8" s="6">
+        <v>4.75</v>
+      </c>
+      <c r="AM8" s="19">
+        <v>4.75</v>
+      </c>
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
@@ -27197,9 +27566,15 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="6"/>
       <c r="AJ9" s="6"/>
-      <c r="AK9" s="6"/>
-      <c r="AL9" s="6"/>
-      <c r="AM9" s="19"/>
+      <c r="AK9" s="6">
+        <v>31.50</v>
+      </c>
+      <c r="AL9" s="6">
+        <v>31.50</v>
+      </c>
+      <c r="AM9" s="19">
+        <v>31.50</v>
+      </c>
       <c r="AN9" s="19"/>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
@@ -27475,7 +27850,7 @@
       <c r="AJ11" s="6"/>
       <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="19"/>
+      <c r="AM11" s="19" t="str"/>
       <c r="AN11" s="19"/>
       <c r="AO11" s="19"/>
       <c r="AP11" s="19"/>
@@ -27587,9 +27962,15 @@
       <c r="AH12" s="10"/>
       <c r="AI12" s="10"/>
       <c r="AJ12" s="10"/>
-      <c r="AK12" s="10"/>
-      <c r="AL12" s="10"/>
-      <c r="AM12" s="20"/>
+      <c r="AK12" s="10">
+        <v>16.00</v>
+      </c>
+      <c r="AL12" s="10">
+        <v>16.00</v>
+      </c>
+      <c r="AM12" s="20">
+        <v>16.00</v>
+      </c>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20"/>
@@ -27674,9 +28055,15 @@
       <c r="AH13" s="10"/>
       <c r="AI13" s="10"/>
       <c r="AJ13" s="10"/>
-      <c r="AK13" s="10"/>
-      <c r="AL13" s="10"/>
-      <c r="AM13" s="20"/>
+      <c r="AK13" s="10">
+        <v>4.75</v>
+      </c>
+      <c r="AL13" s="10">
+        <v>4.75</v>
+      </c>
+      <c r="AM13" s="20">
+        <v>4.75</v>
+      </c>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
@@ -27792,9 +28179,15 @@
       <c r="AH14" s="10"/>
       <c r="AI14" s="10"/>
       <c r="AJ14" s="10"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="10"/>
-      <c r="AM14" s="20"/>
+      <c r="AK14" s="10">
+        <v>18.00</v>
+      </c>
+      <c r="AL14" s="10">
+        <v>18.00</v>
+      </c>
+      <c r="AM14" s="20">
+        <v>23.50</v>
+      </c>
       <c r="AN14" s="38"/>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
@@ -27913,9 +28306,15 @@
       <c r="AH15" s="10"/>
       <c r="AI15" s="10"/>
       <c r="AJ15" s="10"/>
-      <c r="AK15" s="10"/>
-      <c r="AL15" s="10"/>
-      <c r="AM15" s="20"/>
+      <c r="AK15" s="10">
+        <v>17.50</v>
+      </c>
+      <c r="AL15" s="10">
+        <v>17.50</v>
+      </c>
+      <c r="AM15" s="20">
+        <v>17.50</v>
+      </c>
       <c r="AN15" s="38"/>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
@@ -28034,7 +28433,9 @@
       <c r="AJ16" s="10"/>
       <c r="AK16" s="10"/>
       <c r="AL16" s="10"/>
-      <c r="AM16" s="20"/>
+      <c r="AM16" s="20">
+        <v>22.25</v>
+      </c>
       <c r="AN16" s="38"/>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
@@ -28153,9 +28554,15 @@
       <c r="AH17" s="10"/>
       <c r="AI17" s="10"/>
       <c r="AJ17" s="10"/>
-      <c r="AK17" s="10"/>
-      <c r="AL17" s="10"/>
-      <c r="AM17" s="20"/>
+      <c r="AK17" s="10">
+        <v>27.50</v>
+      </c>
+      <c r="AL17" s="10">
+        <v>27.50</v>
+      </c>
+      <c r="AM17" s="20">
+        <v>27.50</v>
+      </c>
       <c r="AN17" s="38"/>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20"/>
@@ -28252,7 +28659,7 @@
       <c r="AJ18" s="10"/>
       <c r="AK18" s="10"/>
       <c r="AL18" s="10"/>
-      <c r="AM18" s="20"/>
+      <c r="AM18" s="20" t="str"/>
       <c r="AN18" s="38"/>
       <c r="AO18" s="20"/>
       <c r="AP18" s="20"/>
@@ -28371,9 +28778,15 @@
       <c r="AH19" s="10"/>
       <c r="AI19" s="10"/>
       <c r="AJ19" s="10"/>
-      <c r="AK19" s="10"/>
-      <c r="AL19" s="10"/>
-      <c r="AM19" s="20"/>
+      <c r="AK19" s="10">
+        <v>7.25</v>
+      </c>
+      <c r="AL19" s="10">
+        <v>7.25</v>
+      </c>
+      <c r="AM19" s="20">
+        <v>7.25</v>
+      </c>
       <c r="AN19" s="38"/>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
@@ -28490,9 +28903,15 @@
       <c r="AH20" s="10"/>
       <c r="AI20" s="10"/>
       <c r="AJ20" s="10"/>
-      <c r="AK20" s="10"/>
-      <c r="AL20" s="10"/>
-      <c r="AM20" s="37"/>
+      <c r="AK20" s="10">
+        <v>32.50</v>
+      </c>
+      <c r="AL20" s="10">
+        <v>32.50</v>
+      </c>
+      <c r="AM20" s="37">
+        <v>32.50</v>
+      </c>
       <c r="AN20" s="37"/>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
@@ -28609,9 +29028,15 @@
       <c r="AH21" s="35"/>
       <c r="AI21" s="35"/>
       <c r="AJ21" s="35"/>
-      <c r="AK21" s="35"/>
-      <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
+      <c r="AK21" s="35">
+        <v>3.00</v>
+      </c>
+      <c r="AL21" s="35">
+        <v>3.00</v>
+      </c>
+      <c r="AM21" s="35">
+        <v>3.00</v>
+      </c>
       <c r="AN21" s="35"/>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
@@ -28730,9 +29155,15 @@
       <c r="AH22" s="35"/>
       <c r="AI22" s="35"/>
       <c r="AJ22" s="35"/>
-      <c r="AK22" s="35"/>
-      <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
+      <c r="AK22" s="35">
+        <v>19.00</v>
+      </c>
+      <c r="AL22" s="35">
+        <v>19.00</v>
+      </c>
+      <c r="AM22" s="35">
+        <v>19.00</v>
+      </c>
       <c r="AN22" s="35"/>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
@@ -29008,7 +29439,7 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
-      <c r="AM24" s="19"/>
+      <c r="AM24" s="19" t="str"/>
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
       <c r="AP24" s="19"/>
@@ -29122,9 +29553,15 @@
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
       <c r="AJ25" s="6"/>
-      <c r="AK25" s="6"/>
-      <c r="AL25" s="6"/>
-      <c r="AM25" s="19"/>
+      <c r="AK25" s="6">
+        <v>23.75</v>
+      </c>
+      <c r="AL25" s="6">
+        <v>23.75</v>
+      </c>
+      <c r="AM25" s="19">
+        <v>23.75</v>
+      </c>
       <c r="AN25" s="19"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
@@ -29234,9 +29671,15 @@
       <c r="AH26" s="10"/>
       <c r="AI26" s="10"/>
       <c r="AJ26" s="10"/>
-      <c r="AK26" s="10"/>
-      <c r="AL26" s="10"/>
-      <c r="AM26" s="20"/>
+      <c r="AK26" s="10">
+        <v>26.00</v>
+      </c>
+      <c r="AL26" s="10">
+        <v>26.00</v>
+      </c>
+      <c r="AM26" s="20">
+        <v>26.00</v>
+      </c>
       <c r="AN26" s="38"/>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
@@ -29353,9 +29796,15 @@
       <c r="AH27" s="10"/>
       <c r="AI27" s="10"/>
       <c r="AJ27" s="10"/>
-      <c r="AK27" s="10"/>
-      <c r="AL27" s="10"/>
-      <c r="AM27" s="20"/>
+      <c r="AK27" s="10">
+        <v>11.00</v>
+      </c>
+      <c r="AL27" s="10">
+        <v>11.00</v>
+      </c>
+      <c r="AM27" s="20">
+        <v>11.00</v>
+      </c>
       <c r="AN27" s="38"/>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
@@ -29468,7 +29917,9 @@
       <c r="AJ28" s="10"/>
       <c r="AK28" s="10"/>
       <c r="AL28" s="10"/>
-      <c r="AM28" s="20"/>
+      <c r="AM28" s="20">
+        <v>35.25</v>
+      </c>
       <c r="AN28" s="38"/>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
@@ -29576,9 +30027,15 @@
       <c r="AH29" s="10"/>
       <c r="AI29" s="10"/>
       <c r="AJ29" s="10"/>
-      <c r="AK29" s="10"/>
-      <c r="AL29" s="10"/>
-      <c r="AM29" s="20"/>
+      <c r="AK29" s="10">
+        <v>4.50</v>
+      </c>
+      <c r="AL29" s="10">
+        <v>4.50</v>
+      </c>
+      <c r="AM29" s="20">
+        <v>4.50</v>
+      </c>
       <c r="AN29" s="38"/>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
@@ -29692,9 +30149,15 @@
       <c r="AH30" s="10"/>
       <c r="AI30" s="10"/>
       <c r="AJ30" s="10"/>
-      <c r="AK30" s="10"/>
-      <c r="AL30" s="10"/>
-      <c r="AM30" s="20"/>
+      <c r="AK30" s="10">
+        <v>18.50</v>
+      </c>
+      <c r="AL30" s="10">
+        <v>18.50</v>
+      </c>
+      <c r="AM30" s="20">
+        <v>18.50</v>
+      </c>
       <c r="AN30" s="38"/>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
@@ -29809,7 +30272,7 @@
       <c r="AJ31" s="10"/>
       <c r="AK31" s="10"/>
       <c r="AL31" s="10"/>
-      <c r="AM31" s="20"/>
+      <c r="AM31" s="20" t="str"/>
       <c r="AN31" s="38"/>
       <c r="AO31" s="20"/>
       <c r="AP31" s="20"/>
@@ -29928,9 +30391,15 @@
       <c r="AH32" s="10"/>
       <c r="AI32" s="10"/>
       <c r="AJ32" s="10"/>
-      <c r="AK32" s="10"/>
-      <c r="AL32" s="10"/>
-      <c r="AM32" s="20"/>
+      <c r="AK32" s="10">
+        <v>13.00</v>
+      </c>
+      <c r="AL32" s="10">
+        <v>13.00</v>
+      </c>
+      <c r="AM32" s="20">
+        <v>13.00</v>
+      </c>
       <c r="AN32" s="38"/>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
@@ -30043,9 +30512,15 @@
       <c r="AH33" s="10"/>
       <c r="AI33" s="10"/>
       <c r="AJ33" s="10"/>
-      <c r="AK33" s="10"/>
-      <c r="AL33" s="10"/>
-      <c r="AM33" s="20"/>
+      <c r="AK33" s="10">
+        <v>15.25</v>
+      </c>
+      <c r="AL33" s="10">
+        <v>15.25</v>
+      </c>
+      <c r="AM33" s="20">
+        <v>15.25</v>
+      </c>
       <c r="AN33" s="38"/>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
@@ -30162,9 +30637,15 @@
       <c r="AH34" s="35"/>
       <c r="AI34" s="35"/>
       <c r="AJ34" s="35"/>
-      <c r="AK34" s="35"/>
-      <c r="AL34" s="35"/>
-      <c r="AM34" s="35"/>
+      <c r="AK34" s="35">
+        <v>1.00</v>
+      </c>
+      <c r="AL34" s="35">
+        <v>1.00</v>
+      </c>
+      <c r="AM34" s="35">
+        <v>1.00</v>
+      </c>
       <c r="AN34" s="35"/>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
@@ -30283,9 +30764,15 @@
       <c r="AH35" s="35"/>
       <c r="AI35" s="35"/>
       <c r="AJ35" s="35"/>
-      <c r="AK35" s="35"/>
-      <c r="AL35" s="35"/>
-      <c r="AM35" s="35"/>
+      <c r="AK35" s="35">
+        <v>35.00</v>
+      </c>
+      <c r="AL35" s="35">
+        <v>35.00</v>
+      </c>
+      <c r="AM35" s="35">
+        <v>35.00</v>
+      </c>
       <c r="AN35" s="35"/>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
@@ -30561,7 +31048,7 @@
       <c r="AJ37" s="10"/>
       <c r="AK37" s="10"/>
       <c r="AL37" s="10"/>
-      <c r="AM37" s="20"/>
+      <c r="AM37" s="20" t="str"/>
       <c r="AN37" s="20"/>
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
@@ -30651,7 +31138,7 @@
       <c r="AJ38" s="23"/>
       <c r="AK38" s="23"/>
       <c r="AL38" s="23"/>
-      <c r="AM38" s="23"/>
+      <c r="AM38" s="23" t="str"/>
       <c r="AN38" s="23"/>
       <c r="AO38" s="23"/>
       <c r="AP38" s="23"/>
@@ -30927,7 +31414,7 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
-      <c r="AM40" s="19"/>
+      <c r="AM40" s="19" t="str"/>
       <c r="AN40" s="19"/>
       <c r="AO40" s="19"/>
       <c r="AP40" s="19"/>
@@ -31043,9 +31530,15 @@
       <c r="AH41" s="10"/>
       <c r="AI41" s="10"/>
       <c r="AJ41" s="10"/>
-      <c r="AK41" s="10"/>
-      <c r="AL41" s="10"/>
-      <c r="AM41" s="20"/>
+      <c r="AK41" s="10">
+        <v>30.00</v>
+      </c>
+      <c r="AL41" s="10">
+        <v>30.00</v>
+      </c>
+      <c r="AM41" s="20">
+        <v>30.00</v>
+      </c>
       <c r="AN41" s="38"/>
       <c r="AO41" s="20"/>
       <c r="AP41" s="20"/>
@@ -31160,9 +31653,15 @@
       <c r="AH42" s="10"/>
       <c r="AI42" s="10"/>
       <c r="AJ42" s="10"/>
-      <c r="AK42" s="10"/>
-      <c r="AL42" s="10"/>
-      <c r="AM42" s="20"/>
+      <c r="AK42" s="10">
+        <v>3.00</v>
+      </c>
+      <c r="AL42" s="10">
+        <v>3.00</v>
+      </c>
+      <c r="AM42" s="20">
+        <v>3.00</v>
+      </c>
       <c r="AN42" s="38"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
@@ -31231,7 +31730,7 @@
       <c r="AJ43" s="10"/>
       <c r="AK43" s="10"/>
       <c r="AL43" s="10"/>
-      <c r="AM43" s="20"/>
+      <c r="AM43" s="20" t="str"/>
       <c r="AN43" s="38"/>
       <c r="AO43" s="20"/>
       <c r="AP43" s="20"/>
@@ -31339,9 +31838,15 @@
       <c r="AH44" s="10"/>
       <c r="AI44" s="10"/>
       <c r="AJ44" s="10"/>
-      <c r="AK44" s="10"/>
-      <c r="AL44" s="10"/>
-      <c r="AM44" s="20"/>
+      <c r="AK44" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="AL44" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="AM44" s="20">
+        <v>0.75</v>
+      </c>
       <c r="AN44" s="38"/>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
@@ -31420,7 +31925,7 @@
       <c r="AJ45" s="10"/>
       <c r="AK45" s="10"/>
       <c r="AL45" s="10"/>
-      <c r="AM45" s="20"/>
+      <c r="AM45" s="20" t="str"/>
       <c r="AN45" s="38"/>
       <c r="AO45" s="20"/>
       <c r="AP45" s="20"/>
@@ -31536,9 +32041,15 @@
       <c r="AH46" s="37"/>
       <c r="AI46" s="37"/>
       <c r="AJ46" s="37"/>
-      <c r="AK46" s="37"/>
-      <c r="AL46" s="37"/>
-      <c r="AM46" s="37"/>
+      <c r="AK46" s="37">
+        <v>23.00</v>
+      </c>
+      <c r="AL46" s="37">
+        <v>23.00</v>
+      </c>
+      <c r="AM46" s="37">
+        <v>23.00</v>
+      </c>
       <c r="AN46" s="37"/>
       <c r="AO46" s="37"/>
       <c r="AP46" s="37"/>
@@ -31814,7 +32325,7 @@
       <c r="AJ48" s="16"/>
       <c r="AK48" s="16"/>
       <c r="AL48" s="16"/>
-      <c r="AM48" s="16"/>
+      <c r="AM48" s="16" t="str"/>
       <c r="AN48" s="16"/>
       <c r="AO48" s="16"/>
       <c r="AP48" s="16"/>
@@ -32087,7 +32598,7 @@
       <c r="AJ50" s="6"/>
       <c r="AK50" s="6"/>
       <c r="AL50" s="6"/>
-      <c r="AM50" s="19"/>
+      <c r="AM50" s="19" t="str"/>
       <c r="AN50" s="19"/>
       <c r="AO50" s="19"/>
       <c r="AP50" s="19"/>
@@ -32201,9 +32712,15 @@
       <c r="AH51" s="10"/>
       <c r="AI51" s="10"/>
       <c r="AJ51" s="10"/>
-      <c r="AK51" s="10"/>
-      <c r="AL51" s="10"/>
-      <c r="AM51" s="20"/>
+      <c r="AK51" s="10">
+        <v>35.75</v>
+      </c>
+      <c r="AL51" s="10">
+        <v>35.75</v>
+      </c>
+      <c r="AM51" s="20">
+        <v>35.75</v>
+      </c>
       <c r="AN51" s="20"/>
       <c r="AO51" s="20"/>
       <c r="AP51" s="20"/>
@@ -32324,7 +32841,9 @@
       <c r="AJ52" s="10"/>
       <c r="AK52" s="10"/>
       <c r="AL52" s="10"/>
-      <c r="AM52" s="20"/>
+      <c r="AM52" s="20">
+        <v>33.00</v>
+      </c>
       <c r="AN52" s="20"/>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
@@ -32439,9 +32958,15 @@
       <c r="AH53" s="10"/>
       <c r="AI53" s="10"/>
       <c r="AJ53" s="10"/>
-      <c r="AK53" s="10"/>
-      <c r="AL53" s="10"/>
-      <c r="AM53" s="20"/>
+      <c r="AK53" s="10">
+        <v>40.00</v>
+      </c>
+      <c r="AL53" s="10">
+        <v>40.00</v>
+      </c>
+      <c r="AM53" s="20">
+        <v>40.00</v>
+      </c>
       <c r="AN53" s="20"/>
       <c r="AO53" s="20"/>
       <c r="AP53" s="20"/>
@@ -32717,7 +33242,7 @@
       <c r="AJ55" s="6"/>
       <c r="AK55" s="6"/>
       <c r="AL55" s="6"/>
-      <c r="AM55" s="19"/>
+      <c r="AM55" s="19" t="str"/>
       <c r="BB55" s="6"/>
     </row>
     <row ht="25" r="56" spans="1:54">
@@ -32813,9 +33338,15 @@
       <c r="AH56" s="6"/>
       <c r="AI56" s="6"/>
       <c r="AJ56" s="6"/>
-      <c r="AK56" s="6"/>
-      <c r="AL56" s="6"/>
-      <c r="AM56" s="19"/>
+      <c r="AK56" s="6">
+        <v>32.75</v>
+      </c>
+      <c r="AL56" s="6">
+        <v>32.75</v>
+      </c>
+      <c r="AM56" s="19">
+        <v>32.75</v>
+      </c>
       <c r="AN56" s="37"/>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37"/>
@@ -32907,7 +33438,7 @@
       <c r="AJ57" s="23"/>
       <c r="AK57" s="23"/>
       <c r="AL57" s="23"/>
-      <c r="AM57" s="31"/>
+      <c r="AM57" s="31" t="str"/>
       <c r="AN57" s="35"/>
       <c r="AO57" s="35"/>
       <c r="AP57" s="35"/>
@@ -33179,7 +33710,7 @@
       <c r="AJ59" s="16"/>
       <c r="AK59" s="16"/>
       <c r="AL59" s="16"/>
-      <c r="AM59" s="16"/>
+      <c r="AM59" s="16" t="str"/>
       <c r="AN59" s="16"/>
       <c r="AO59" s="16"/>
       <c r="AP59" s="16"/>
@@ -33282,9 +33813,15 @@
         <v>9</v>
       </c>
       <c r="AJ60" s="37"/>
-      <c r="AK60" s="10"/>
-      <c r="AL60" s="10"/>
-      <c r="AM60" s="106"/>
+      <c r="AK60" s="10">
+        <v>10.00</v>
+      </c>
+      <c r="AL60" s="10">
+        <v>10.00</v>
+      </c>
+      <c r="AM60" s="106">
+        <v>10.00</v>
+      </c>
       <c r="AN60" s="106"/>
       <c r="AO60" s="106"/>
       <c r="AP60" s="106"/>
@@ -33374,9 +33911,15 @@
         <v>3.00</v>
       </c>
       <c r="AJ61" s="37"/>
-      <c r="AK61" s="10"/>
-      <c r="AL61" s="10"/>
-      <c r="AM61" s="106"/>
+      <c r="AK61" s="10">
+        <v>20.00</v>
+      </c>
+      <c r="AL61" s="10">
+        <v>20.00</v>
+      </c>
+      <c r="AM61" s="106">
+        <v>20.00</v>
+      </c>
       <c r="AN61" s="106"/>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
@@ -33462,9 +34005,15 @@
         <v>11.25</v>
       </c>
       <c r="AJ62" s="37"/>
-      <c r="AK62" s="10"/>
-      <c r="AL62" s="10"/>
-      <c r="AM62" s="106"/>
+      <c r="AK62" s="10">
+        <v>18.50</v>
+      </c>
+      <c r="AL62" s="10">
+        <v>18.50</v>
+      </c>
+      <c r="AM62" s="106">
+        <v>18.50</v>
+      </c>
       <c r="AN62" s="106"/>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
@@ -33537,7 +34086,7 @@
       <c r="AA63" s="117"/>
       <c r="AB63" s="117"/>
       <c r="AJ63" s="37"/>
-      <c r="AM63" s="106"/>
+      <c r="AM63" s="106" t="str"/>
       <c r="AN63" s="106"/>
       <c r="AO63" s="106"/>
       <c r="AP63" s="106"/>
@@ -33652,7 +34201,15 @@
         <v>16.00</v>
       </c>
       <c r="AJ64" s="37"/>
-      <c r="AM64" s="106"/>
+      <c r="AK64">
+        <v>25.50</v>
+      </c>
+      <c r="AL64">
+        <v>25.50</v>
+      </c>
+      <c r="AM64" s="106">
+        <v>25.50</v>
+      </c>
       <c r="AN64" s="106"/>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
@@ -33767,7 +34324,15 @@
         <v>7.50</v>
       </c>
       <c r="AJ65" s="37"/>
-      <c r="AM65" s="106"/>
+      <c r="AK65">
+        <v>15.00</v>
+      </c>
+      <c r="AL65">
+        <v>15.00</v>
+      </c>
+      <c r="AM65" s="106">
+        <v>15.00</v>
+      </c>
       <c r="AN65" s="106"/>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
@@ -34399,14 +34964,30 @@
       <c r="AE2" s="1" t="str">
         <v>22.07-28.07.19</v>
       </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="AF2" s="1" t="str">
+        <v>29.07-04.08.19</v>
+      </c>
+      <c r="AG2" s="1" t="str">
+        <v>05.08-11.08.19</v>
+      </c>
+      <c r="AH2" s="1" t="str">
+        <v>12.08-18.08.19</v>
+      </c>
+      <c r="AI2" s="1" t="str">
+        <v>19.08-25.08.19</v>
+      </c>
+      <c r="AJ2" s="1" t="str">
+        <v>26.08-01.09.19</v>
+      </c>
+      <c r="AK2" s="1" t="str">
+        <v>02.09-08.09.19</v>
+      </c>
+      <c r="AL2" s="1" t="str">
+        <v>09.09-15.09.19</v>
+      </c>
+      <c r="AM2" s="1" t="str">
+        <v>16.09-22.09.19</v>
+      </c>
       <c r="AN2" s="18"/>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
@@ -34589,7 +35170,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="AM4" t="str"/>
+    </row>
     <row ht="34" r="5" spans="1:54">
       <c r="A5" s="2" t="s">
         <v>2</v>
@@ -34906,7 +35489,9 @@
       </c>
       <c r="BB6" s="3"/>
     </row>
-    <row r="7"/>
+    <row r="7">
+      <c r="AM7" t="str"/>
+    </row>
     <row ht="25" r="8" spans="1:54">
       <c r="A8" s="5" t="s">
         <v>104</v>
@@ -35000,7 +35585,7 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="19"/>
+      <c r="AM8" s="19" t="str"/>
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
@@ -35109,7 +35694,7 @@
       <c r="AJ9" s="6"/>
       <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="19"/>
+      <c r="AM9" s="19" t="str"/>
       <c r="AN9" s="19"/>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
@@ -35385,7 +35970,7 @@
       <c r="AJ11" s="6"/>
       <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="19"/>
+      <c r="AM11" s="19" t="str"/>
       <c r="AN11" s="19"/>
       <c r="AO11" s="19"/>
       <c r="AP11" s="19"/>
@@ -35493,7 +36078,7 @@
       <c r="AJ12" s="10"/>
       <c r="AK12" s="10"/>
       <c r="AL12" s="10"/>
-      <c r="AM12" s="20"/>
+      <c r="AM12" s="20" t="str"/>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20"/>
@@ -35566,9 +36151,15 @@
       <c r="AH13" s="10"/>
       <c r="AI13" s="10"/>
       <c r="AJ13" s="10"/>
-      <c r="AK13" s="10"/>
-      <c r="AL13" s="10"/>
-      <c r="AM13" s="20"/>
+      <c r="AK13" s="10">
+        <v>24.00</v>
+      </c>
+      <c r="AL13" s="10">
+        <v>24.00</v>
+      </c>
+      <c r="AM13" s="20">
+        <v>24.00</v>
+      </c>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
@@ -35674,7 +36265,7 @@
       <c r="AJ14" s="10"/>
       <c r="AK14" s="10"/>
       <c r="AL14" s="10"/>
-      <c r="AM14" s="20"/>
+      <c r="AM14" s="20" t="str"/>
       <c r="AN14" s="38"/>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
@@ -35785,7 +36376,7 @@
       <c r="AJ15" s="10"/>
       <c r="AK15" s="10"/>
       <c r="AL15" s="10"/>
-      <c r="AM15" s="20"/>
+      <c r="AM15" s="20" t="str"/>
       <c r="AN15" s="38"/>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
@@ -35896,7 +36487,7 @@
       <c r="AJ16" s="10"/>
       <c r="AK16" s="10"/>
       <c r="AL16" s="10"/>
-      <c r="AM16" s="20"/>
+      <c r="AM16" s="20" t="str"/>
       <c r="AN16" s="38"/>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
@@ -36005,7 +36596,7 @@
       <c r="AJ17" s="10"/>
       <c r="AK17" s="10"/>
       <c r="AL17" s="10"/>
-      <c r="AM17" s="20"/>
+      <c r="AM17" s="20" t="str"/>
       <c r="AN17" s="38"/>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20"/>
@@ -36104,7 +36695,7 @@
       <c r="AJ18" s="10"/>
       <c r="AK18" s="10"/>
       <c r="AL18" s="10"/>
-      <c r="AM18" s="20"/>
+      <c r="AM18" s="20" t="str"/>
       <c r="AN18" s="38"/>
       <c r="AO18" s="20"/>
       <c r="AP18" s="20"/>
@@ -36215,9 +36806,15 @@
       <c r="AH19" s="10"/>
       <c r="AI19" s="10"/>
       <c r="AJ19" s="10"/>
-      <c r="AK19" s="10"/>
-      <c r="AL19" s="10"/>
-      <c r="AM19" s="20"/>
+      <c r="AK19" s="10">
+        <v>8.00</v>
+      </c>
+      <c r="AL19" s="10">
+        <v>8.00</v>
+      </c>
+      <c r="AM19" s="20">
+        <v>8.00</v>
+      </c>
       <c r="AN19" s="38"/>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
@@ -36330,9 +36927,15 @@
       <c r="AH20" s="10"/>
       <c r="AI20" s="10"/>
       <c r="AJ20" s="10"/>
-      <c r="AK20" s="10"/>
-      <c r="AL20" s="10"/>
-      <c r="AM20" s="37"/>
+      <c r="AK20" s="10">
+        <v>4.00</v>
+      </c>
+      <c r="AL20" s="10">
+        <v>4.00</v>
+      </c>
+      <c r="AM20" s="37">
+        <v>4.00</v>
+      </c>
       <c r="AN20" s="37"/>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
@@ -36439,9 +37042,15 @@
       <c r="AH21" s="35"/>
       <c r="AI21" s="35"/>
       <c r="AJ21" s="35"/>
-      <c r="AK21" s="35"/>
-      <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
+      <c r="AK21" s="35">
+        <v>7.00</v>
+      </c>
+      <c r="AL21" s="35">
+        <v>7.00</v>
+      </c>
+      <c r="AM21" s="35">
+        <v>7.00</v>
+      </c>
       <c r="AN21" s="35"/>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
@@ -36550,7 +37159,7 @@
       <c r="AJ22" s="35"/>
       <c r="AK22" s="35"/>
       <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
+      <c r="AM22" s="35" t="str"/>
       <c r="AN22" s="35"/>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
@@ -36826,7 +37435,7 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
-      <c r="AM24" s="19"/>
+      <c r="AM24" s="19" t="str"/>
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
       <c r="AP24" s="19"/>
@@ -36932,7 +37541,7 @@
       <c r="AJ25" s="6"/>
       <c r="AK25" s="6"/>
       <c r="AL25" s="6"/>
-      <c r="AM25" s="19"/>
+      <c r="AM25" s="19" t="str"/>
       <c r="AN25" s="19"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
@@ -37042,7 +37651,7 @@
       <c r="AJ26" s="10"/>
       <c r="AK26" s="10"/>
       <c r="AL26" s="10"/>
-      <c r="AM26" s="20"/>
+      <c r="AM26" s="20" t="str"/>
       <c r="AN26" s="38"/>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
@@ -37149,7 +37758,7 @@
       <c r="AJ27" s="10"/>
       <c r="AK27" s="10"/>
       <c r="AL27" s="10"/>
-      <c r="AM27" s="20"/>
+      <c r="AM27" s="20" t="str"/>
       <c r="AN27" s="38"/>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
@@ -37260,7 +37869,7 @@
       <c r="AJ28" s="10"/>
       <c r="AK28" s="10"/>
       <c r="AL28" s="10"/>
-      <c r="AM28" s="20"/>
+      <c r="AM28" s="20" t="str"/>
       <c r="AN28" s="38"/>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
@@ -37370,9 +37979,15 @@
       <c r="AH29" s="10"/>
       <c r="AI29" s="10"/>
       <c r="AJ29" s="10"/>
-      <c r="AK29" s="10"/>
-      <c r="AL29" s="10"/>
-      <c r="AM29" s="20"/>
+      <c r="AK29" s="10">
+        <v>5.00</v>
+      </c>
+      <c r="AL29" s="10">
+        <v>5.00</v>
+      </c>
+      <c r="AM29" s="20">
+        <v>5.00</v>
+      </c>
       <c r="AN29" s="38"/>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
@@ -37478,7 +38093,7 @@
       <c r="AJ30" s="10"/>
       <c r="AK30" s="10"/>
       <c r="AL30" s="10"/>
-      <c r="AM30" s="20"/>
+      <c r="AM30" s="20" t="str"/>
       <c r="AN30" s="38"/>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
@@ -37591,9 +38206,15 @@
       <c r="AH31" s="10"/>
       <c r="AI31" s="10"/>
       <c r="AJ31" s="10"/>
-      <c r="AK31" s="10"/>
-      <c r="AL31" s="10"/>
-      <c r="AM31" s="20"/>
+      <c r="AK31" s="10">
+        <v>40.00</v>
+      </c>
+      <c r="AL31" s="10">
+        <v>40.00</v>
+      </c>
+      <c r="AM31" s="20">
+        <v>40.00</v>
+      </c>
       <c r="AN31" s="38"/>
       <c r="AO31" s="20"/>
       <c r="AP31" s="20"/>
@@ -37700,7 +38321,7 @@
       <c r="AJ32" s="10"/>
       <c r="AK32" s="10"/>
       <c r="AL32" s="10"/>
-      <c r="AM32" s="20"/>
+      <c r="AM32" s="20" t="str"/>
       <c r="AN32" s="38"/>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
@@ -37811,9 +38432,15 @@
       <c r="AH33" s="10"/>
       <c r="AI33" s="10"/>
       <c r="AJ33" s="10"/>
-      <c r="AK33" s="10"/>
-      <c r="AL33" s="10"/>
-      <c r="AM33" s="20"/>
+      <c r="AK33" s="10">
+        <v>8.00</v>
+      </c>
+      <c r="AL33" s="10">
+        <v>8.00</v>
+      </c>
+      <c r="AM33" s="20">
+        <v>8.00</v>
+      </c>
       <c r="AN33" s="38"/>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
@@ -37922,7 +38549,7 @@
       <c r="AJ34" s="35"/>
       <c r="AK34" s="35"/>
       <c r="AL34" s="35"/>
-      <c r="AM34" s="35"/>
+      <c r="AM34" s="35" t="str"/>
       <c r="AN34" s="35"/>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
@@ -38029,7 +38656,7 @@
       <c r="AJ35" s="35"/>
       <c r="AK35" s="35"/>
       <c r="AL35" s="35"/>
-      <c r="AM35" s="35"/>
+      <c r="AM35" s="35" t="str"/>
       <c r="AN35" s="35"/>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
@@ -38305,7 +38932,7 @@
       <c r="AJ37" s="10"/>
       <c r="AK37" s="10"/>
       <c r="AL37" s="10"/>
-      <c r="AM37" s="20"/>
+      <c r="AM37" s="20" t="str"/>
       <c r="AN37" s="20"/>
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
@@ -38395,7 +39022,7 @@
       <c r="AJ38" s="23"/>
       <c r="AK38" s="23"/>
       <c r="AL38" s="23"/>
-      <c r="AM38" s="23"/>
+      <c r="AM38" s="23" t="str"/>
       <c r="AN38" s="23"/>
       <c r="AO38" s="23"/>
       <c r="AP38" s="23"/>
@@ -38671,7 +39298,7 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
-      <c r="AM40" s="19"/>
+      <c r="AM40" s="19" t="str"/>
       <c r="AN40" s="19"/>
       <c r="AO40" s="19"/>
       <c r="AP40" s="19"/>
@@ -38781,7 +39408,7 @@
       <c r="AJ41" s="10"/>
       <c r="AK41" s="10"/>
       <c r="AL41" s="10"/>
-      <c r="AM41" s="20"/>
+      <c r="AM41" s="20" t="str"/>
       <c r="AN41" s="38"/>
       <c r="AO41" s="20"/>
       <c r="AP41" s="20"/>
@@ -38888,7 +39515,7 @@
       <c r="AJ42" s="10"/>
       <c r="AK42" s="10"/>
       <c r="AL42" s="10"/>
-      <c r="AM42" s="20"/>
+      <c r="AM42" s="20" t="str"/>
       <c r="AN42" s="38"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
@@ -38949,7 +39576,7 @@
       <c r="AJ43" s="10"/>
       <c r="AK43" s="10"/>
       <c r="AL43" s="10"/>
-      <c r="AM43" s="20"/>
+      <c r="AM43" s="20" t="str"/>
       <c r="AN43" s="38"/>
       <c r="AO43" s="20"/>
       <c r="AP43" s="20"/>
@@ -39057,7 +39684,7 @@
       <c r="AJ44" s="10"/>
       <c r="AK44" s="10"/>
       <c r="AL44" s="10"/>
-      <c r="AM44" s="20"/>
+      <c r="AM44" s="20" t="str"/>
       <c r="AN44" s="38"/>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
@@ -39136,7 +39763,7 @@
       <c r="AJ45" s="10"/>
       <c r="AK45" s="10"/>
       <c r="AL45" s="10"/>
-      <c r="AM45" s="20"/>
+      <c r="AM45" s="20" t="str"/>
       <c r="AN45" s="38"/>
       <c r="AO45" s="20"/>
       <c r="AP45" s="20"/>
@@ -39240,7 +39867,7 @@
       <c r="AJ46" s="37"/>
       <c r="AK46" s="37"/>
       <c r="AL46" s="37"/>
-      <c r="AM46" s="37"/>
+      <c r="AM46" s="37" t="str"/>
       <c r="AN46" s="37"/>
       <c r="AO46" s="37"/>
       <c r="AP46" s="37"/>
@@ -39516,7 +40143,7 @@
       <c r="AJ48" s="16"/>
       <c r="AK48" s="16"/>
       <c r="AL48" s="16"/>
-      <c r="AM48" s="16"/>
+      <c r="AM48" s="16" t="str"/>
       <c r="AN48" s="16"/>
       <c r="AO48" s="16"/>
       <c r="AP48" s="16"/>
@@ -39789,7 +40416,7 @@
       <c r="AJ50" s="6"/>
       <c r="AK50" s="6"/>
       <c r="AL50" s="6"/>
-      <c r="AM50" s="19"/>
+      <c r="AM50" s="19" t="str"/>
       <c r="AN50" s="19"/>
       <c r="AO50" s="19"/>
       <c r="AP50" s="19"/>
@@ -39895,7 +40522,7 @@
       <c r="AJ51" s="10"/>
       <c r="AK51" s="10"/>
       <c r="AL51" s="10"/>
-      <c r="AM51" s="20"/>
+      <c r="AM51" s="20" t="str"/>
       <c r="AN51" s="20"/>
       <c r="AO51" s="20"/>
       <c r="AP51" s="20"/>
@@ -40006,7 +40633,7 @@
       <c r="AJ52" s="10"/>
       <c r="AK52" s="10"/>
       <c r="AL52" s="10"/>
-      <c r="AM52" s="20"/>
+      <c r="AM52" s="20" t="str"/>
       <c r="AN52" s="20"/>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
@@ -40123,7 +40750,7 @@
       <c r="AJ53" s="10"/>
       <c r="AK53" s="10"/>
       <c r="AL53" s="10"/>
-      <c r="AM53" s="20"/>
+      <c r="AM53" s="20" t="str"/>
       <c r="AN53" s="20"/>
       <c r="AO53" s="20"/>
       <c r="AP53" s="20"/>
@@ -40399,7 +41026,7 @@
       <c r="AJ55" s="6"/>
       <c r="AK55" s="6"/>
       <c r="AL55" s="6"/>
-      <c r="AM55" s="19"/>
+      <c r="AM55" s="19" t="str"/>
       <c r="BB55" s="6"/>
     </row>
     <row ht="25" r="56" spans="1:54">
@@ -40495,7 +41122,7 @@
       <c r="AJ56" s="6"/>
       <c r="AK56" s="6"/>
       <c r="AL56" s="6"/>
-      <c r="AM56" s="19"/>
+      <c r="AM56" s="19" t="str"/>
       <c r="AN56" s="37"/>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37"/>
@@ -40587,7 +41214,7 @@
       <c r="AJ57" s="23"/>
       <c r="AK57" s="23"/>
       <c r="AL57" s="23"/>
-      <c r="AM57" s="31"/>
+      <c r="AM57" s="31" t="str"/>
       <c r="AN57" s="35"/>
       <c r="AO57" s="35"/>
       <c r="AP57" s="35"/>
@@ -40859,7 +41486,7 @@
       <c r="AJ59" s="16"/>
       <c r="AK59" s="16"/>
       <c r="AL59" s="16"/>
-      <c r="AM59" s="16"/>
+      <c r="AM59" s="16" t="str"/>
       <c r="AN59" s="16"/>
       <c r="AO59" s="16"/>
       <c r="AP59" s="16"/>
@@ -40961,7 +41588,7 @@
       <c r="AJ60" s="37"/>
       <c r="AK60" s="10"/>
       <c r="AL60" s="10"/>
-      <c r="AM60" s="106"/>
+      <c r="AM60" s="106" t="str"/>
       <c r="AN60" s="106"/>
       <c r="AO60" s="106"/>
       <c r="AP60" s="106"/>
@@ -41045,9 +41672,15 @@
         <v>8.00</v>
       </c>
       <c r="AJ61" s="37"/>
-      <c r="AK61" s="10"/>
-      <c r="AL61" s="10"/>
-      <c r="AM61" s="106"/>
+      <c r="AK61" s="10">
+        <v>16.00</v>
+      </c>
+      <c r="AL61" s="10">
+        <v>16.00</v>
+      </c>
+      <c r="AM61" s="106">
+        <v>16.00</v>
+      </c>
       <c r="AN61" s="106"/>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
@@ -41115,9 +41748,15 @@
         <v>4</v>
       </c>
       <c r="AJ62" s="37"/>
-      <c r="AK62" s="10"/>
-      <c r="AL62" s="10"/>
-      <c r="AM62" s="106"/>
+      <c r="AK62" s="10">
+        <v>4.00</v>
+      </c>
+      <c r="AL62" s="10">
+        <v>4.00</v>
+      </c>
+      <c r="AM62" s="106">
+        <v>4.00</v>
+      </c>
       <c r="AN62" s="106"/>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
@@ -41188,7 +41827,7 @@
       <c r="W63" s="117"/>
       <c r="X63" s="117"/>
       <c r="AJ63" s="37"/>
-      <c r="AM63" s="106"/>
+      <c r="AM63" s="106" t="str"/>
       <c r="AN63" s="106"/>
       <c r="AO63" s="106"/>
       <c r="AP63" s="106"/>
@@ -41282,7 +41921,7 @@
         <v>0</v>
       </c>
       <c r="AJ64" s="37"/>
-      <c r="AM64" s="106"/>
+      <c r="AM64" s="106" t="str"/>
       <c r="AN64" s="106"/>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
@@ -41379,7 +42018,7 @@
         <v>16</v>
       </c>
       <c r="AJ65" s="37"/>
-      <c r="AM65" s="106"/>
+      <c r="AM65" s="106" t="str"/>
       <c r="AN65" s="106"/>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
@@ -42014,14 +42653,30 @@
       <c r="AE2" s="1" t="str">
         <v>22.07-28.07.19</v>
       </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="AF2" s="1" t="str">
+        <v>29.07-04.08.19</v>
+      </c>
+      <c r="AG2" s="1" t="str">
+        <v>05.08-11.08.19</v>
+      </c>
+      <c r="AH2" s="1" t="str">
+        <v>12.08-18.08.19</v>
+      </c>
+      <c r="AI2" s="1" t="str">
+        <v>19.08-25.08.19</v>
+      </c>
+      <c r="AJ2" s="1" t="str">
+        <v>26.08-01.09.19</v>
+      </c>
+      <c r="AK2" s="1" t="str">
+        <v>02.09-08.09.19</v>
+      </c>
+      <c r="AL2" s="1" t="str">
+        <v>09.09-15.09.19</v>
+      </c>
+      <c r="AM2" s="1" t="str">
+        <v>16.09-22.09.19</v>
+      </c>
       <c r="AN2" s="18"/>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
@@ -42204,7 +42859,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="AM4" t="str"/>
+    </row>
     <row ht="34" r="5" spans="1:54">
       <c r="A5" s="2" t="s">
         <v>2</v>
@@ -42521,7 +43178,9 @@
       </c>
       <c r="BB6" s="3"/>
     </row>
-    <row r="7"/>
+    <row r="7">
+      <c r="AM7" t="str"/>
+    </row>
     <row ht="25" r="8" spans="1:54">
       <c r="A8" s="5" t="s">
         <v>104</v>
@@ -42611,7 +43270,7 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="19"/>
+      <c r="AM8" s="19" t="str"/>
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
@@ -42722,7 +43381,7 @@
       <c r="AJ9" s="6"/>
       <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="19"/>
+      <c r="AM9" s="19" t="str"/>
       <c r="AN9" s="19"/>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
@@ -42998,7 +43657,7 @@
       <c r="AJ11" s="6"/>
       <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="19"/>
+      <c r="AM11" s="19" t="str"/>
       <c r="AN11" s="19"/>
       <c r="AO11" s="19"/>
       <c r="AP11" s="19"/>
@@ -43102,7 +43761,7 @@
       <c r="AJ12" s="10"/>
       <c r="AK12" s="10"/>
       <c r="AL12" s="10"/>
-      <c r="AM12" s="20"/>
+      <c r="AM12" s="20" t="str"/>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20"/>
@@ -43175,7 +43834,7 @@
       <c r="AJ13" s="10"/>
       <c r="AK13" s="10"/>
       <c r="AL13" s="10"/>
-      <c r="AM13" s="20"/>
+      <c r="AM13" s="20" t="str"/>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
@@ -43285,7 +43944,7 @@
       <c r="AJ14" s="10"/>
       <c r="AK14" s="10"/>
       <c r="AL14" s="10"/>
-      <c r="AM14" s="20"/>
+      <c r="AM14" s="20" t="str"/>
       <c r="AN14" s="38"/>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
@@ -43398,7 +44057,7 @@
       <c r="AJ15" s="10"/>
       <c r="AK15" s="10"/>
       <c r="AL15" s="10"/>
-      <c r="AM15" s="20"/>
+      <c r="AM15" s="20" t="str"/>
       <c r="AN15" s="38"/>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
@@ -43507,7 +44166,7 @@
       <c r="AJ16" s="10"/>
       <c r="AK16" s="10"/>
       <c r="AL16" s="10"/>
-      <c r="AM16" s="20"/>
+      <c r="AM16" s="20" t="str"/>
       <c r="AN16" s="38"/>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
@@ -43614,7 +44273,7 @@
       <c r="AJ17" s="10"/>
       <c r="AK17" s="10"/>
       <c r="AL17" s="10"/>
-      <c r="AM17" s="20"/>
+      <c r="AM17" s="20" t="str"/>
       <c r="AN17" s="38"/>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20"/>
@@ -43711,7 +44370,7 @@
       <c r="AJ18" s="10"/>
       <c r="AK18" s="10"/>
       <c r="AL18" s="10"/>
-      <c r="AM18" s="20"/>
+      <c r="AM18" s="20" t="str"/>
       <c r="AN18" s="38"/>
       <c r="AO18" s="20"/>
       <c r="AP18" s="20"/>
@@ -43818,7 +44477,7 @@
       <c r="AJ19" s="10"/>
       <c r="AK19" s="10"/>
       <c r="AL19" s="10"/>
-      <c r="AM19" s="20"/>
+      <c r="AM19" s="20" t="str"/>
       <c r="AN19" s="38"/>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
@@ -43925,7 +44584,7 @@
       <c r="AJ20" s="10"/>
       <c r="AK20" s="10"/>
       <c r="AL20" s="10"/>
-      <c r="AM20" s="37"/>
+      <c r="AM20" s="37" t="str"/>
       <c r="AN20" s="37"/>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
@@ -44040,7 +44699,7 @@
       <c r="AJ21" s="35"/>
       <c r="AK21" s="35"/>
       <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
+      <c r="AM21" s="35" t="str"/>
       <c r="AN21" s="35"/>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
@@ -44147,9 +44806,15 @@
       <c r="AH22" s="35"/>
       <c r="AI22" s="35"/>
       <c r="AJ22" s="35"/>
-      <c r="AK22" s="35"/>
-      <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
+      <c r="AK22" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="AL22" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="AM22" s="35">
+        <v>0.25</v>
+      </c>
       <c r="AN22" s="35"/>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
@@ -44425,7 +45090,7 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
-      <c r="AM24" s="19"/>
+      <c r="AM24" s="19" t="str"/>
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
       <c r="AP24" s="19"/>
@@ -44529,7 +45194,7 @@
       <c r="AJ25" s="6"/>
       <c r="AK25" s="6"/>
       <c r="AL25" s="6"/>
-      <c r="AM25" s="19"/>
+      <c r="AM25" s="19" t="str"/>
       <c r="AN25" s="19"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
@@ -44637,9 +45302,15 @@
       <c r="AH26" s="10"/>
       <c r="AI26" s="10"/>
       <c r="AJ26" s="10"/>
-      <c r="AK26" s="10"/>
-      <c r="AL26" s="10"/>
-      <c r="AM26" s="20"/>
+      <c r="AK26" s="10">
+        <v>1.00</v>
+      </c>
+      <c r="AL26" s="10">
+        <v>1.00</v>
+      </c>
+      <c r="AM26" s="20">
+        <v>1.00</v>
+      </c>
       <c r="AN26" s="38"/>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
@@ -44754,7 +45425,7 @@
       <c r="AJ27" s="10"/>
       <c r="AK27" s="10"/>
       <c r="AL27" s="10"/>
-      <c r="AM27" s="20"/>
+      <c r="AM27" s="20" t="str"/>
       <c r="AN27" s="38"/>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
@@ -44861,7 +45532,7 @@
       <c r="AJ28" s="10"/>
       <c r="AK28" s="10"/>
       <c r="AL28" s="10"/>
-      <c r="AM28" s="20"/>
+      <c r="AM28" s="20" t="str"/>
       <c r="AN28" s="38"/>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
@@ -44965,7 +45636,7 @@
       <c r="AJ29" s="10"/>
       <c r="AK29" s="10"/>
       <c r="AL29" s="10"/>
-      <c r="AM29" s="20"/>
+      <c r="AM29" s="20" t="str"/>
       <c r="AN29" s="38"/>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
@@ -45069,7 +45740,7 @@
       <c r="AJ30" s="10"/>
       <c r="AK30" s="10"/>
       <c r="AL30" s="10"/>
-      <c r="AM30" s="20"/>
+      <c r="AM30" s="20" t="str"/>
       <c r="AN30" s="38"/>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
@@ -45176,7 +45847,7 @@
       <c r="AJ31" s="10"/>
       <c r="AK31" s="10"/>
       <c r="AL31" s="10"/>
-      <c r="AM31" s="20"/>
+      <c r="AM31" s="20" t="str"/>
       <c r="AN31" s="38"/>
       <c r="AO31" s="20"/>
       <c r="AP31" s="20"/>
@@ -45285,7 +45956,7 @@
       <c r="AJ32" s="10"/>
       <c r="AK32" s="10"/>
       <c r="AL32" s="10"/>
-      <c r="AM32" s="20"/>
+      <c r="AM32" s="20" t="str"/>
       <c r="AN32" s="38"/>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
@@ -45394,7 +46065,7 @@
       <c r="AJ33" s="10"/>
       <c r="AK33" s="10"/>
       <c r="AL33" s="10"/>
-      <c r="AM33" s="20"/>
+      <c r="AM33" s="20" t="str"/>
       <c r="AN33" s="38"/>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
@@ -45503,7 +46174,7 @@
       <c r="AJ34" s="35"/>
       <c r="AK34" s="35"/>
       <c r="AL34" s="35"/>
-      <c r="AM34" s="35"/>
+      <c r="AM34" s="35" t="str"/>
       <c r="AN34" s="35"/>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
@@ -45612,7 +46283,7 @@
       <c r="AJ35" s="35"/>
       <c r="AK35" s="35"/>
       <c r="AL35" s="35"/>
-      <c r="AM35" s="35"/>
+      <c r="AM35" s="35" t="str"/>
       <c r="AN35" s="35"/>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
@@ -45888,7 +46559,7 @@
       <c r="AJ37" s="10"/>
       <c r="AK37" s="10"/>
       <c r="AL37" s="10"/>
-      <c r="AM37" s="20"/>
+      <c r="AM37" s="20" t="str"/>
       <c r="AN37" s="20"/>
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
@@ -45978,7 +46649,7 @@
       <c r="AJ38" s="23"/>
       <c r="AK38" s="23"/>
       <c r="AL38" s="23"/>
-      <c r="AM38" s="23"/>
+      <c r="AM38" s="23" t="str"/>
       <c r="AN38" s="23"/>
       <c r="AO38" s="23"/>
       <c r="AP38" s="23"/>
@@ -46254,7 +46925,7 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
-      <c r="AM40" s="19"/>
+      <c r="AM40" s="19" t="str"/>
       <c r="AN40" s="19"/>
       <c r="AO40" s="19"/>
       <c r="AP40" s="19"/>
@@ -46360,7 +47031,7 @@
       <c r="AJ41" s="10"/>
       <c r="AK41" s="10"/>
       <c r="AL41" s="10"/>
-      <c r="AM41" s="20"/>
+      <c r="AM41" s="20" t="str"/>
       <c r="AN41" s="38"/>
       <c r="AO41" s="20"/>
       <c r="AP41" s="20"/>
@@ -46467,7 +47138,7 @@
       <c r="AJ42" s="10"/>
       <c r="AK42" s="10"/>
       <c r="AL42" s="10"/>
-      <c r="AM42" s="20"/>
+      <c r="AM42" s="20" t="str"/>
       <c r="AN42" s="38"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
@@ -46528,7 +47199,7 @@
       <c r="AJ43" s="10"/>
       <c r="AK43" s="10"/>
       <c r="AL43" s="10"/>
-      <c r="AM43" s="20"/>
+      <c r="AM43" s="20" t="str"/>
       <c r="AN43" s="38"/>
       <c r="AO43" s="20"/>
       <c r="AP43" s="20"/>
@@ -46632,7 +47303,7 @@
       <c r="AJ44" s="10"/>
       <c r="AK44" s="10"/>
       <c r="AL44" s="10"/>
-      <c r="AM44" s="20"/>
+      <c r="AM44" s="20" t="str"/>
       <c r="AN44" s="38"/>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
@@ -46711,7 +47382,7 @@
       <c r="AJ45" s="10"/>
       <c r="AK45" s="10"/>
       <c r="AL45" s="10"/>
-      <c r="AM45" s="20"/>
+      <c r="AM45" s="20" t="str"/>
       <c r="AN45" s="38"/>
       <c r="AO45" s="20"/>
       <c r="AP45" s="20"/>
@@ -46815,7 +47486,7 @@
       <c r="AJ46" s="37"/>
       <c r="AK46" s="37"/>
       <c r="AL46" s="37"/>
-      <c r="AM46" s="37"/>
+      <c r="AM46" s="37" t="str"/>
       <c r="AN46" s="37"/>
       <c r="AO46" s="37"/>
       <c r="AP46" s="37"/>
@@ -47091,7 +47762,7 @@
       <c r="AJ48" s="16"/>
       <c r="AK48" s="16"/>
       <c r="AL48" s="16"/>
-      <c r="AM48" s="16"/>
+      <c r="AM48" s="16" t="str"/>
       <c r="AN48" s="16"/>
       <c r="AO48" s="16"/>
       <c r="AP48" s="16"/>
@@ -47364,7 +48035,7 @@
       <c r="AJ50" s="6"/>
       <c r="AK50" s="6"/>
       <c r="AL50" s="6"/>
-      <c r="AM50" s="19"/>
+      <c r="AM50" s="19" t="str"/>
       <c r="AN50" s="19"/>
       <c r="AO50" s="19"/>
       <c r="AP50" s="19"/>
@@ -47470,7 +48141,7 @@
       <c r="AJ51" s="10"/>
       <c r="AK51" s="10"/>
       <c r="AL51" s="10"/>
-      <c r="AM51" s="20"/>
+      <c r="AM51" s="20" t="str"/>
       <c r="AN51" s="20"/>
       <c r="AO51" s="20"/>
       <c r="AP51" s="20"/>
@@ -47577,7 +48248,7 @@
       <c r="AJ52" s="10"/>
       <c r="AK52" s="10"/>
       <c r="AL52" s="10"/>
-      <c r="AM52" s="20"/>
+      <c r="AM52" s="20" t="str"/>
       <c r="AN52" s="20"/>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
@@ -47684,7 +48355,7 @@
       <c r="AJ53" s="10"/>
       <c r="AK53" s="10"/>
       <c r="AL53" s="10"/>
-      <c r="AM53" s="20"/>
+      <c r="AM53" s="20" t="str"/>
       <c r="AN53" s="20"/>
       <c r="AO53" s="20"/>
       <c r="AP53" s="20"/>
@@ -47960,7 +48631,7 @@
       <c r="AJ55" s="6"/>
       <c r="AK55" s="6"/>
       <c r="AL55" s="6"/>
-      <c r="AM55" s="19"/>
+      <c r="AM55" s="19" t="str"/>
       <c r="BB55" s="6"/>
     </row>
     <row ht="25" r="56" spans="1:54">
@@ -48052,7 +48723,7 @@
       <c r="AJ56" s="6"/>
       <c r="AK56" s="6"/>
       <c r="AL56" s="6"/>
-      <c r="AM56" s="19"/>
+      <c r="AM56" s="19" t="str"/>
       <c r="AN56" s="37"/>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37"/>
@@ -48144,7 +48815,7 @@
       <c r="AJ57" s="23"/>
       <c r="AK57" s="23"/>
       <c r="AL57" s="23"/>
-      <c r="AM57" s="31"/>
+      <c r="AM57" s="31" t="str"/>
       <c r="AN57" s="35"/>
       <c r="AO57" s="35"/>
       <c r="AP57" s="35"/>
@@ -48416,7 +49087,7 @@
       <c r="AJ59" s="16"/>
       <c r="AK59" s="16"/>
       <c r="AL59" s="16"/>
-      <c r="AM59" s="16"/>
+      <c r="AM59" s="16" t="str"/>
       <c r="AN59" s="16"/>
       <c r="AO59" s="16"/>
       <c r="AP59" s="16"/>
@@ -48512,7 +49183,7 @@
       <c r="AJ60" s="37"/>
       <c r="AK60" s="10"/>
       <c r="AL60" s="10"/>
-      <c r="AM60" s="106"/>
+      <c r="AM60" s="106" t="str"/>
       <c r="AN60" s="106"/>
       <c r="AO60" s="106"/>
       <c r="AP60" s="106"/>
@@ -48586,7 +49257,7 @@
       <c r="AJ61" s="37"/>
       <c r="AK61" s="10"/>
       <c r="AL61" s="10"/>
-      <c r="AM61" s="106"/>
+      <c r="AM61" s="106" t="str"/>
       <c r="AN61" s="106"/>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
@@ -48656,7 +49327,7 @@
       <c r="AJ62" s="37"/>
       <c r="AK62" s="10"/>
       <c r="AL62" s="10"/>
-      <c r="AM62" s="106"/>
+      <c r="AM62" s="106" t="str"/>
       <c r="AN62" s="106"/>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
@@ -48725,7 +49396,7 @@
       <c r="W63" s="117"/>
       <c r="X63" s="117"/>
       <c r="AJ63" s="37"/>
-      <c r="AM63" s="106"/>
+      <c r="AM63" s="106" t="str"/>
       <c r="AN63" s="106"/>
       <c r="AO63" s="106"/>
       <c r="AP63" s="106"/>
@@ -48822,7 +49493,7 @@
         <v>5</v>
       </c>
       <c r="AJ64" s="37"/>
-      <c r="AM64" s="106"/>
+      <c r="AM64" s="106" t="str"/>
       <c r="AN64" s="106"/>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
@@ -48928,7 +49599,15 @@
         <v>2.00</v>
       </c>
       <c r="AJ65" s="37"/>
-      <c r="AM65" s="106"/>
+      <c r="AK65">
+        <v>0.50</v>
+      </c>
+      <c r="AL65">
+        <v>0.50</v>
+      </c>
+      <c r="AM65" s="106">
+        <v>0.50</v>
+      </c>
       <c r="AN65" s="106"/>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
@@ -49562,14 +50241,30 @@
       <c r="AE2" s="1" t="str">
         <v>22.07-28.07.19</v>
       </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="AF2" s="1" t="str">
+        <v>29.07-04.08.19</v>
+      </c>
+      <c r="AG2" s="1" t="str">
+        <v>05.08-11.08.19</v>
+      </c>
+      <c r="AH2" s="1" t="str">
+        <v>12.08-18.08.19</v>
+      </c>
+      <c r="AI2" s="1" t="str">
+        <v>19.08-25.08.19</v>
+      </c>
+      <c r="AJ2" s="1" t="str">
+        <v>26.08-01.09.19</v>
+      </c>
+      <c r="AK2" s="1" t="str">
+        <v>02.09-08.09.19</v>
+      </c>
+      <c r="AL2" s="1" t="str">
+        <v>09.09-15.09.19</v>
+      </c>
+      <c r="AM2" s="1" t="str">
+        <v>16.09-22.09.19</v>
+      </c>
       <c r="AN2" s="18"/>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
@@ -49768,6 +50463,7 @@
       <c r="S4" s="105" t="s">
         <v>95</v>
       </c>
+      <c r="AM4" t="str"/>
     </row>
     <row ht="34" r="5" spans="1:54">
       <c r="A5" s="2" t="s">
@@ -50085,7 +50781,9 @@
       </c>
       <c r="BB6" s="3"/>
     </row>
-    <row r="7"/>
+    <row r="7">
+      <c r="AM7" t="str"/>
+    </row>
     <row ht="25" r="8" spans="1:54">
       <c r="A8" s="5" t="s">
         <v>104</v>
@@ -50139,7 +50837,7 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="19"/>
+      <c r="AM8" s="19" t="str"/>
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
@@ -50212,7 +50910,7 @@
       <c r="AJ9" s="6"/>
       <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="19"/>
+      <c r="AM9" s="19" t="str"/>
       <c r="AN9" s="19"/>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
@@ -50488,7 +51186,7 @@
       <c r="AJ11" s="6"/>
       <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="19"/>
+      <c r="AM11" s="19" t="str"/>
       <c r="AN11" s="19"/>
       <c r="AO11" s="19"/>
       <c r="AP11" s="19"/>
@@ -50558,7 +51256,7 @@
       <c r="AJ12" s="10"/>
       <c r="AK12" s="10"/>
       <c r="AL12" s="10"/>
-      <c r="AM12" s="20"/>
+      <c r="AM12" s="20" t="str"/>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20"/>
@@ -50623,7 +51321,7 @@
       <c r="AJ13" s="10"/>
       <c r="AK13" s="10"/>
       <c r="AL13" s="10"/>
-      <c r="AM13" s="20"/>
+      <c r="AM13" s="20" t="str"/>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
@@ -50693,7 +51391,7 @@
       <c r="AJ14" s="10"/>
       <c r="AK14" s="10"/>
       <c r="AL14" s="10"/>
-      <c r="AM14" s="20"/>
+      <c r="AM14" s="20" t="str"/>
       <c r="AN14" s="38"/>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
@@ -50766,7 +51464,7 @@
       <c r="AJ15" s="10"/>
       <c r="AK15" s="10"/>
       <c r="AL15" s="10"/>
-      <c r="AM15" s="20"/>
+      <c r="AM15" s="20" t="str"/>
       <c r="AN15" s="38"/>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
@@ -50839,7 +51537,7 @@
       <c r="AJ16" s="10"/>
       <c r="AK16" s="10"/>
       <c r="AL16" s="10"/>
-      <c r="AM16" s="20"/>
+      <c r="AM16" s="20" t="str"/>
       <c r="AN16" s="38"/>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
@@ -50912,7 +51610,7 @@
       <c r="AJ17" s="10"/>
       <c r="AK17" s="10"/>
       <c r="AL17" s="10"/>
-      <c r="AM17" s="20"/>
+      <c r="AM17" s="20" t="str"/>
       <c r="AN17" s="38"/>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20"/>
@@ -50983,7 +51681,7 @@
       <c r="AJ18" s="10"/>
       <c r="AK18" s="10"/>
       <c r="AL18" s="10"/>
-      <c r="AM18" s="20"/>
+      <c r="AM18" s="20" t="str"/>
       <c r="AN18" s="38"/>
       <c r="AO18" s="20"/>
       <c r="AP18" s="20"/>
@@ -51056,7 +51754,7 @@
       <c r="AJ19" s="10"/>
       <c r="AK19" s="10"/>
       <c r="AL19" s="10"/>
-      <c r="AM19" s="20"/>
+      <c r="AM19" s="20" t="str"/>
       <c r="AN19" s="38"/>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
@@ -51129,7 +51827,7 @@
       <c r="AJ20" s="10"/>
       <c r="AK20" s="10"/>
       <c r="AL20" s="10"/>
-      <c r="AM20" s="37"/>
+      <c r="AM20" s="37" t="str"/>
       <c r="AN20" s="37"/>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
@@ -51202,7 +51900,7 @@
       <c r="AJ21" s="35"/>
       <c r="AK21" s="35"/>
       <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
+      <c r="AM21" s="35" t="str"/>
       <c r="AN21" s="35"/>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
@@ -51275,7 +51973,7 @@
       <c r="AJ22" s="35"/>
       <c r="AK22" s="35"/>
       <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
+      <c r="AM22" s="35" t="str"/>
       <c r="AN22" s="35"/>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
@@ -51551,7 +52249,7 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
-      <c r="AM24" s="19"/>
+      <c r="AM24" s="19" t="str"/>
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
       <c r="AP24" s="19"/>
@@ -51621,7 +52319,7 @@
       <c r="AJ25" s="6"/>
       <c r="AK25" s="6"/>
       <c r="AL25" s="6"/>
-      <c r="AM25" s="19"/>
+      <c r="AM25" s="19" t="str"/>
       <c r="AN25" s="19"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
@@ -51691,7 +52389,7 @@
       <c r="AJ26" s="10"/>
       <c r="AK26" s="10"/>
       <c r="AL26" s="10"/>
-      <c r="AM26" s="20"/>
+      <c r="AM26" s="20" t="str"/>
       <c r="AN26" s="38"/>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
@@ -51764,7 +52462,7 @@
       <c r="AJ27" s="10"/>
       <c r="AK27" s="10"/>
       <c r="AL27" s="10"/>
-      <c r="AM27" s="20"/>
+      <c r="AM27" s="20" t="str"/>
       <c r="AN27" s="38"/>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
@@ -51837,7 +52535,7 @@
       <c r="AJ28" s="10"/>
       <c r="AK28" s="10"/>
       <c r="AL28" s="10"/>
-      <c r="AM28" s="20"/>
+      <c r="AM28" s="20" t="str"/>
       <c r="AN28" s="38"/>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
@@ -51907,7 +52605,7 @@
       <c r="AJ29" s="10"/>
       <c r="AK29" s="10"/>
       <c r="AL29" s="10"/>
-      <c r="AM29" s="20"/>
+      <c r="AM29" s="20" t="str"/>
       <c r="AN29" s="38"/>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
@@ -51977,7 +52675,7 @@
       <c r="AJ30" s="10"/>
       <c r="AK30" s="10"/>
       <c r="AL30" s="10"/>
-      <c r="AM30" s="20"/>
+      <c r="AM30" s="20" t="str"/>
       <c r="AN30" s="38"/>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
@@ -52050,7 +52748,7 @@
       <c r="AJ31" s="10"/>
       <c r="AK31" s="10"/>
       <c r="AL31" s="10"/>
-      <c r="AM31" s="20"/>
+      <c r="AM31" s="20" t="str"/>
       <c r="AN31" s="38"/>
       <c r="AO31" s="20"/>
       <c r="AP31" s="20"/>
@@ -52123,7 +52821,7 @@
       <c r="AJ32" s="10"/>
       <c r="AK32" s="10"/>
       <c r="AL32" s="10"/>
-      <c r="AM32" s="20"/>
+      <c r="AM32" s="20" t="str"/>
       <c r="AN32" s="38"/>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
@@ -52196,7 +52894,7 @@
       <c r="AJ33" s="10"/>
       <c r="AK33" s="10"/>
       <c r="AL33" s="10"/>
-      <c r="AM33" s="20"/>
+      <c r="AM33" s="20" t="str"/>
       <c r="AN33" s="38"/>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
@@ -52269,7 +52967,7 @@
       <c r="AJ34" s="35"/>
       <c r="AK34" s="35"/>
       <c r="AL34" s="35"/>
-      <c r="AM34" s="35"/>
+      <c r="AM34" s="35" t="str"/>
       <c r="AN34" s="35"/>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
@@ -52342,7 +53040,7 @@
       <c r="AJ35" s="35"/>
       <c r="AK35" s="35"/>
       <c r="AL35" s="35"/>
-      <c r="AM35" s="35"/>
+      <c r="AM35" s="35" t="str"/>
       <c r="AN35" s="35"/>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
@@ -52618,7 +53316,7 @@
       <c r="AJ37" s="10"/>
       <c r="AK37" s="10"/>
       <c r="AL37" s="10"/>
-      <c r="AM37" s="20"/>
+      <c r="AM37" s="20" t="str"/>
       <c r="AN37" s="20"/>
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
@@ -52682,7 +53380,7 @@
       <c r="AJ38" s="23"/>
       <c r="AK38" s="23"/>
       <c r="AL38" s="23"/>
-      <c r="AM38" s="23"/>
+      <c r="AM38" s="23" t="str"/>
       <c r="AN38" s="23"/>
       <c r="AO38" s="23"/>
       <c r="AP38" s="23"/>
@@ -52958,7 +53656,7 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
-      <c r="AM40" s="19"/>
+      <c r="AM40" s="19" t="str"/>
       <c r="AN40" s="19"/>
       <c r="AO40" s="19"/>
       <c r="AP40" s="19"/>
@@ -53028,7 +53726,7 @@
       <c r="AJ41" s="10"/>
       <c r="AK41" s="10"/>
       <c r="AL41" s="10"/>
-      <c r="AM41" s="20"/>
+      <c r="AM41" s="20" t="str"/>
       <c r="AN41" s="38"/>
       <c r="AO41" s="20"/>
       <c r="AP41" s="20"/>
@@ -53101,7 +53799,7 @@
       <c r="AJ42" s="10"/>
       <c r="AK42" s="10"/>
       <c r="AL42" s="10"/>
-      <c r="AM42" s="20"/>
+      <c r="AM42" s="20" t="str"/>
       <c r="AN42" s="38"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
@@ -53162,7 +53860,7 @@
       <c r="AJ43" s="10"/>
       <c r="AK43" s="10"/>
       <c r="AL43" s="10"/>
-      <c r="AM43" s="20"/>
+      <c r="AM43" s="20" t="str"/>
       <c r="AN43" s="38"/>
       <c r="AO43" s="20"/>
       <c r="AP43" s="20"/>
@@ -53232,7 +53930,7 @@
       <c r="AJ44" s="10"/>
       <c r="AK44" s="10"/>
       <c r="AL44" s="10"/>
-      <c r="AM44" s="20"/>
+      <c r="AM44" s="20" t="str"/>
       <c r="AN44" s="38"/>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
@@ -53301,7 +53999,7 @@
       <c r="AJ45" s="10"/>
       <c r="AK45" s="10"/>
       <c r="AL45" s="10"/>
-      <c r="AM45" s="20"/>
+      <c r="AM45" s="20" t="str"/>
       <c r="AN45" s="38"/>
       <c r="AO45" s="20"/>
       <c r="AP45" s="20"/>
@@ -53371,7 +54069,7 @@
       <c r="AJ46" s="37"/>
       <c r="AK46" s="37"/>
       <c r="AL46" s="37"/>
-      <c r="AM46" s="37"/>
+      <c r="AM46" s="37" t="str"/>
       <c r="AN46" s="37"/>
       <c r="AO46" s="37"/>
       <c r="AP46" s="37"/>
@@ -53647,7 +54345,7 @@
       <c r="AJ48" s="16"/>
       <c r="AK48" s="16"/>
       <c r="AL48" s="16"/>
-      <c r="AM48" s="16"/>
+      <c r="AM48" s="16" t="str"/>
       <c r="AN48" s="16"/>
       <c r="AO48" s="16"/>
       <c r="AP48" s="16"/>
@@ -53920,7 +54618,7 @@
       <c r="AJ50" s="6"/>
       <c r="AK50" s="6"/>
       <c r="AL50" s="6"/>
-      <c r="AM50" s="19"/>
+      <c r="AM50" s="19" t="str"/>
       <c r="AN50" s="19"/>
       <c r="AO50" s="19"/>
       <c r="AP50" s="19"/>
@@ -53990,7 +54688,7 @@
       <c r="AJ51" s="10"/>
       <c r="AK51" s="10"/>
       <c r="AL51" s="10"/>
-      <c r="AM51" s="20"/>
+      <c r="AM51" s="20" t="str"/>
       <c r="AN51" s="20"/>
       <c r="AO51" s="20"/>
       <c r="AP51" s="20"/>
@@ -54063,7 +54761,7 @@
       <c r="AJ52" s="10"/>
       <c r="AK52" s="10"/>
       <c r="AL52" s="10"/>
-      <c r="AM52" s="20"/>
+      <c r="AM52" s="20" t="str"/>
       <c r="AN52" s="20"/>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
@@ -54136,7 +54834,7 @@
       <c r="AJ53" s="10"/>
       <c r="AK53" s="10"/>
       <c r="AL53" s="10"/>
-      <c r="AM53" s="20"/>
+      <c r="AM53" s="20" t="str"/>
       <c r="AN53" s="20"/>
       <c r="AO53" s="20"/>
       <c r="AP53" s="20"/>
@@ -54412,7 +55110,7 @@
       <c r="AJ55" s="6"/>
       <c r="AK55" s="6"/>
       <c r="AL55" s="6"/>
-      <c r="AM55" s="19"/>
+      <c r="AM55" s="19" t="str"/>
       <c r="BB55" s="6"/>
     </row>
     <row ht="25" r="56" spans="1:54">
@@ -54468,7 +55166,7 @@
       <c r="AJ56" s="6"/>
       <c r="AK56" s="6"/>
       <c r="AL56" s="6"/>
-      <c r="AM56" s="19"/>
+      <c r="AM56" s="19" t="str"/>
       <c r="AN56" s="37"/>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37"/>
@@ -54528,7 +55226,7 @@
       <c r="AJ57" s="23"/>
       <c r="AK57" s="23"/>
       <c r="AL57" s="23"/>
-      <c r="AM57" s="31"/>
+      <c r="AM57" s="31" t="str"/>
       <c r="AN57" s="35"/>
       <c r="AO57" s="35"/>
       <c r="AP57" s="35"/>
@@ -54800,7 +55498,7 @@
       <c r="AJ59" s="16"/>
       <c r="AK59" s="16"/>
       <c r="AL59" s="16"/>
-      <c r="AM59" s="16"/>
+      <c r="AM59" s="16" t="str"/>
       <c r="AN59" s="16"/>
       <c r="AO59" s="16"/>
       <c r="AP59" s="16"/>
@@ -54855,7 +55553,7 @@
       <c r="AJ60" s="37"/>
       <c r="AK60" s="10"/>
       <c r="AL60" s="10"/>
-      <c r="AM60" s="106"/>
+      <c r="AM60" s="106" t="str"/>
       <c r="AN60" s="106"/>
       <c r="AO60" s="106"/>
       <c r="AP60" s="106"/>
@@ -54909,7 +55607,7 @@
       <c r="AJ61" s="37"/>
       <c r="AK61" s="10"/>
       <c r="AL61" s="10"/>
-      <c r="AM61" s="106"/>
+      <c r="AM61" s="106" t="str"/>
       <c r="AN61" s="106"/>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
@@ -54960,7 +55658,7 @@
       <c r="AJ62" s="37"/>
       <c r="AK62" s="10"/>
       <c r="AL62" s="10"/>
-      <c r="AM62" s="106"/>
+      <c r="AM62" s="106" t="str"/>
       <c r="AN62" s="106"/>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
@@ -55009,7 +55707,7 @@
       <c r="W63" s="117"/>
       <c r="X63" s="117"/>
       <c r="AJ63" s="37"/>
-      <c r="AM63" s="106"/>
+      <c r="AM63" s="106" t="str"/>
       <c r="AN63" s="106"/>
       <c r="AO63" s="106"/>
       <c r="AP63" s="106"/>
@@ -55065,7 +55763,7 @@
         <v>5</v>
       </c>
       <c r="AJ64" s="37"/>
-      <c r="AM64" s="106"/>
+      <c r="AM64" s="106" t="str"/>
       <c r="AN64" s="106"/>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
@@ -55121,7 +55819,7 @@
         <v>8</v>
       </c>
       <c r="AJ65" s="37"/>
-      <c r="AM65" s="106"/>
+      <c r="AM65" s="106" t="str"/>
       <c r="AN65" s="106"/>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
@@ -55753,14 +56451,30 @@
       <c r="AE2" s="1" t="str">
         <v>22.07-28.07.19</v>
       </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="AF2" s="1" t="str">
+        <v>29.07-04.08.19</v>
+      </c>
+      <c r="AG2" s="1" t="str">
+        <v>05.08-11.08.19</v>
+      </c>
+      <c r="AH2" s="1" t="str">
+        <v>12.08-18.08.19</v>
+      </c>
+      <c r="AI2" s="1" t="str">
+        <v>19.08-25.08.19</v>
+      </c>
+      <c r="AJ2" s="1" t="str">
+        <v>26.08-01.09.19</v>
+      </c>
+      <c r="AK2" s="1" t="str">
+        <v>02.09-08.09.19</v>
+      </c>
+      <c r="AL2" s="1" t="str">
+        <v>09.09-15.09.19</v>
+      </c>
+      <c r="AM2" s="1" t="str">
+        <v>16.09-22.09.19</v>
+      </c>
       <c r="AN2" s="18"/>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
@@ -55943,7 +56657,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="AM4" t="str"/>
+    </row>
     <row ht="34" r="5" spans="1:54">
       <c r="A5" s="2" t="s">
         <v>2</v>
@@ -56260,7 +56976,9 @@
       </c>
       <c r="BB6" s="3"/>
     </row>
-    <row r="7"/>
+    <row r="7">
+      <c r="AM7" t="str"/>
+    </row>
     <row ht="25" r="8" spans="1:54">
       <c r="A8" s="5" t="s">
         <v>104</v>
@@ -56348,7 +57066,7 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="19"/>
+      <c r="AM8" s="19" t="str"/>
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
@@ -56455,7 +57173,7 @@
       <c r="AJ9" s="6"/>
       <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="19"/>
+      <c r="AM9" s="19" t="str"/>
       <c r="AN9" s="19"/>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
@@ -56731,7 +57449,7 @@
       <c r="AJ11" s="6"/>
       <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="19"/>
+      <c r="AM11" s="19" t="str"/>
       <c r="AN11" s="19"/>
       <c r="AO11" s="19"/>
       <c r="AP11" s="19"/>
@@ -56835,7 +57553,7 @@
       <c r="AJ12" s="10"/>
       <c r="AK12" s="10"/>
       <c r="AL12" s="10"/>
-      <c r="AM12" s="20"/>
+      <c r="AM12" s="20" t="str"/>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20"/>
@@ -56906,7 +57624,7 @@
       <c r="AJ13" s="10"/>
       <c r="AK13" s="10"/>
       <c r="AL13" s="10"/>
-      <c r="AM13" s="20"/>
+      <c r="AM13" s="20" t="str"/>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
@@ -57010,7 +57728,7 @@
       <c r="AJ14" s="10"/>
       <c r="AK14" s="10"/>
       <c r="AL14" s="10"/>
-      <c r="AM14" s="20"/>
+      <c r="AM14" s="20" t="str"/>
       <c r="AN14" s="38"/>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
@@ -57117,7 +57835,7 @@
       <c r="AJ15" s="10"/>
       <c r="AK15" s="10"/>
       <c r="AL15" s="10"/>
-      <c r="AM15" s="20"/>
+      <c r="AM15" s="20" t="str"/>
       <c r="AN15" s="38"/>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
@@ -57224,7 +57942,7 @@
       <c r="AJ16" s="10"/>
       <c r="AK16" s="10"/>
       <c r="AL16" s="10"/>
-      <c r="AM16" s="20"/>
+      <c r="AM16" s="20" t="str"/>
       <c r="AN16" s="38"/>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
@@ -57331,7 +58049,7 @@
       <c r="AJ17" s="10"/>
       <c r="AK17" s="10"/>
       <c r="AL17" s="10"/>
-      <c r="AM17" s="20"/>
+      <c r="AM17" s="20" t="str"/>
       <c r="AN17" s="38"/>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20"/>
@@ -57428,7 +58146,7 @@
       <c r="AJ18" s="10"/>
       <c r="AK18" s="10"/>
       <c r="AL18" s="10"/>
-      <c r="AM18" s="20"/>
+      <c r="AM18" s="20" t="str"/>
       <c r="AN18" s="38"/>
       <c r="AO18" s="20"/>
       <c r="AP18" s="20"/>
@@ -57535,7 +58253,7 @@
       <c r="AJ19" s="10"/>
       <c r="AK19" s="10"/>
       <c r="AL19" s="10"/>
-      <c r="AM19" s="20"/>
+      <c r="AM19" s="20" t="str"/>
       <c r="AN19" s="38"/>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
@@ -57642,7 +58360,7 @@
       <c r="AJ20" s="10"/>
       <c r="AK20" s="10"/>
       <c r="AL20" s="10"/>
-      <c r="AM20" s="37"/>
+      <c r="AM20" s="37" t="str"/>
       <c r="AN20" s="37"/>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
@@ -57749,7 +58467,7 @@
       <c r="AJ21" s="35"/>
       <c r="AK21" s="35"/>
       <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
+      <c r="AM21" s="35" t="str"/>
       <c r="AN21" s="35"/>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
@@ -57856,7 +58574,7 @@
       <c r="AJ22" s="35"/>
       <c r="AK22" s="35"/>
       <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
+      <c r="AM22" s="35" t="str"/>
       <c r="AN22" s="35"/>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
@@ -58132,7 +58850,7 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
-      <c r="AM24" s="19"/>
+      <c r="AM24" s="19" t="str"/>
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
       <c r="AP24" s="19"/>
@@ -58236,7 +58954,7 @@
       <c r="AJ25" s="6"/>
       <c r="AK25" s="6"/>
       <c r="AL25" s="6"/>
-      <c r="AM25" s="19"/>
+      <c r="AM25" s="19" t="str"/>
       <c r="AN25" s="19"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
@@ -58340,7 +59058,7 @@
       <c r="AJ26" s="10"/>
       <c r="AK26" s="10"/>
       <c r="AL26" s="10"/>
-      <c r="AM26" s="20"/>
+      <c r="AM26" s="20" t="str"/>
       <c r="AN26" s="38"/>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
@@ -58451,7 +59169,7 @@
       <c r="AJ27" s="10"/>
       <c r="AK27" s="10"/>
       <c r="AL27" s="10"/>
-      <c r="AM27" s="20"/>
+      <c r="AM27" s="20" t="str"/>
       <c r="AN27" s="38"/>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
@@ -58558,7 +59276,7 @@
       <c r="AJ28" s="10"/>
       <c r="AK28" s="10"/>
       <c r="AL28" s="10"/>
-      <c r="AM28" s="20"/>
+      <c r="AM28" s="20" t="str"/>
       <c r="AN28" s="38"/>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
@@ -58662,7 +59380,7 @@
       <c r="AJ29" s="10"/>
       <c r="AK29" s="10"/>
       <c r="AL29" s="10"/>
-      <c r="AM29" s="20"/>
+      <c r="AM29" s="20" t="str"/>
       <c r="AN29" s="38"/>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
@@ -58766,7 +59484,7 @@
       <c r="AJ30" s="10"/>
       <c r="AK30" s="10"/>
       <c r="AL30" s="10"/>
-      <c r="AM30" s="20"/>
+      <c r="AM30" s="20" t="str"/>
       <c r="AN30" s="38"/>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
@@ -58873,7 +59591,7 @@
       <c r="AJ31" s="10"/>
       <c r="AK31" s="10"/>
       <c r="AL31" s="10"/>
-      <c r="AM31" s="20"/>
+      <c r="AM31" s="20" t="str"/>
       <c r="AN31" s="38"/>
       <c r="AO31" s="20"/>
       <c r="AP31" s="20"/>
@@ -58980,7 +59698,7 @@
       <c r="AJ32" s="10"/>
       <c r="AK32" s="10"/>
       <c r="AL32" s="10"/>
-      <c r="AM32" s="20"/>
+      <c r="AM32" s="20" t="str"/>
       <c r="AN32" s="38"/>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
@@ -59087,7 +59805,7 @@
       <c r="AJ33" s="10"/>
       <c r="AK33" s="10"/>
       <c r="AL33" s="10"/>
-      <c r="AM33" s="20"/>
+      <c r="AM33" s="20" t="str"/>
       <c r="AN33" s="38"/>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
@@ -59194,7 +59912,7 @@
       <c r="AJ34" s="35"/>
       <c r="AK34" s="35"/>
       <c r="AL34" s="35"/>
-      <c r="AM34" s="35"/>
+      <c r="AM34" s="35" t="str"/>
       <c r="AN34" s="35"/>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
@@ -59301,7 +60019,7 @@
       <c r="AJ35" s="35"/>
       <c r="AK35" s="35"/>
       <c r="AL35" s="35"/>
-      <c r="AM35" s="35"/>
+      <c r="AM35" s="35" t="str"/>
       <c r="AN35" s="35"/>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
@@ -59577,7 +60295,7 @@
       <c r="AJ37" s="10"/>
       <c r="AK37" s="10"/>
       <c r="AL37" s="10"/>
-      <c r="AM37" s="20"/>
+      <c r="AM37" s="20" t="str"/>
       <c r="AN37" s="20"/>
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
@@ -59667,7 +60385,7 @@
       <c r="AJ38" s="23"/>
       <c r="AK38" s="23"/>
       <c r="AL38" s="23"/>
-      <c r="AM38" s="23"/>
+      <c r="AM38" s="23" t="str"/>
       <c r="AN38" s="23"/>
       <c r="AO38" s="23"/>
       <c r="AP38" s="23"/>
@@ -59943,7 +60661,7 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
-      <c r="AM40" s="19"/>
+      <c r="AM40" s="19" t="str"/>
       <c r="AN40" s="19"/>
       <c r="AO40" s="19"/>
       <c r="AP40" s="19"/>
@@ -60047,7 +60765,7 @@
       <c r="AJ41" s="10"/>
       <c r="AK41" s="10"/>
       <c r="AL41" s="10"/>
-      <c r="AM41" s="20"/>
+      <c r="AM41" s="20" t="str"/>
       <c r="AN41" s="38"/>
       <c r="AO41" s="20"/>
       <c r="AP41" s="20"/>
@@ -60158,7 +60876,7 @@
       <c r="AJ42" s="10"/>
       <c r="AK42" s="10"/>
       <c r="AL42" s="10"/>
-      <c r="AM42" s="20"/>
+      <c r="AM42" s="20" t="str"/>
       <c r="AN42" s="38"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
@@ -60219,7 +60937,7 @@
       <c r="AJ43" s="10"/>
       <c r="AK43" s="10"/>
       <c r="AL43" s="10"/>
-      <c r="AM43" s="20"/>
+      <c r="AM43" s="20" t="str"/>
       <c r="AN43" s="38"/>
       <c r="AO43" s="20"/>
       <c r="AP43" s="20"/>
@@ -60323,7 +61041,7 @@
       <c r="AJ44" s="10"/>
       <c r="AK44" s="10"/>
       <c r="AL44" s="10"/>
-      <c r="AM44" s="20"/>
+      <c r="AM44" s="20" t="str"/>
       <c r="AN44" s="38"/>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
@@ -60402,7 +61120,7 @@
       <c r="AJ45" s="10"/>
       <c r="AK45" s="10"/>
       <c r="AL45" s="10"/>
-      <c r="AM45" s="20"/>
+      <c r="AM45" s="20" t="str"/>
       <c r="AN45" s="38"/>
       <c r="AO45" s="20"/>
       <c r="AP45" s="20"/>
@@ -60506,7 +61224,7 @@
       <c r="AJ46" s="37"/>
       <c r="AK46" s="37"/>
       <c r="AL46" s="37"/>
-      <c r="AM46" s="37"/>
+      <c r="AM46" s="37" t="str"/>
       <c r="AN46" s="37"/>
       <c r="AO46" s="37"/>
       <c r="AP46" s="37"/>
@@ -60782,7 +61500,7 @@
       <c r="AJ48" s="16"/>
       <c r="AK48" s="16"/>
       <c r="AL48" s="16"/>
-      <c r="AM48" s="16"/>
+      <c r="AM48" s="16" t="str"/>
       <c r="AN48" s="16"/>
       <c r="AO48" s="16"/>
       <c r="AP48" s="16"/>
@@ -61055,7 +61773,7 @@
       <c r="AJ50" s="6"/>
       <c r="AK50" s="6"/>
       <c r="AL50" s="6"/>
-      <c r="AM50" s="19"/>
+      <c r="AM50" s="19" t="str"/>
       <c r="AN50" s="19"/>
       <c r="AO50" s="19"/>
       <c r="AP50" s="19"/>
@@ -61159,7 +61877,7 @@
       <c r="AJ51" s="10"/>
       <c r="AK51" s="10"/>
       <c r="AL51" s="10"/>
-      <c r="AM51" s="20"/>
+      <c r="AM51" s="20" t="str"/>
       <c r="AN51" s="20"/>
       <c r="AO51" s="20"/>
       <c r="AP51" s="20"/>
@@ -61266,7 +61984,7 @@
       <c r="AJ52" s="10"/>
       <c r="AK52" s="10"/>
       <c r="AL52" s="10"/>
-      <c r="AM52" s="20"/>
+      <c r="AM52" s="20" t="str"/>
       <c r="AN52" s="20"/>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
@@ -61373,7 +62091,7 @@
       <c r="AJ53" s="10"/>
       <c r="AK53" s="10"/>
       <c r="AL53" s="10"/>
-      <c r="AM53" s="20"/>
+      <c r="AM53" s="20" t="str"/>
       <c r="AN53" s="20"/>
       <c r="AO53" s="20"/>
       <c r="AP53" s="20"/>
@@ -61649,7 +62367,7 @@
       <c r="AJ55" s="6"/>
       <c r="AK55" s="6"/>
       <c r="AL55" s="6"/>
-      <c r="AM55" s="19"/>
+      <c r="AM55" s="19" t="str"/>
       <c r="BB55" s="6"/>
     </row>
     <row ht="25" r="56" spans="1:54">
@@ -61739,7 +62457,7 @@
       <c r="AJ56" s="6"/>
       <c r="AK56" s="6"/>
       <c r="AL56" s="6"/>
-      <c r="AM56" s="19"/>
+      <c r="AM56" s="19" t="str"/>
       <c r="AN56" s="37"/>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37"/>
@@ -61831,7 +62549,7 @@
       <c r="AJ57" s="23"/>
       <c r="AK57" s="23"/>
       <c r="AL57" s="23"/>
-      <c r="AM57" s="31"/>
+      <c r="AM57" s="31" t="str"/>
       <c r="AN57" s="35"/>
       <c r="AO57" s="35"/>
       <c r="AP57" s="35"/>
@@ -62103,7 +62821,7 @@
       <c r="AJ59" s="16"/>
       <c r="AK59" s="16"/>
       <c r="AL59" s="16"/>
-      <c r="AM59" s="16"/>
+      <c r="AM59" s="16" t="str"/>
       <c r="AN59" s="16"/>
       <c r="AO59" s="16"/>
       <c r="AP59" s="16"/>
@@ -62196,7 +62914,7 @@
       <c r="AJ60" s="37"/>
       <c r="AK60" s="10"/>
       <c r="AL60" s="10"/>
-      <c r="AM60" s="106"/>
+      <c r="AM60" s="106" t="str"/>
       <c r="AN60" s="106"/>
       <c r="AO60" s="106"/>
       <c r="AP60" s="106"/>
@@ -62270,7 +62988,7 @@
       <c r="AJ61" s="37"/>
       <c r="AK61" s="10"/>
       <c r="AL61" s="10"/>
-      <c r="AM61" s="106"/>
+      <c r="AM61" s="106" t="str"/>
       <c r="AN61" s="106"/>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
@@ -62343,7 +63061,7 @@
       <c r="AJ62" s="37"/>
       <c r="AK62" s="10"/>
       <c r="AL62" s="10"/>
-      <c r="AM62" s="106"/>
+      <c r="AM62" s="106" t="str"/>
       <c r="AN62" s="106"/>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
@@ -62412,7 +63130,7 @@
       <c r="W63" s="117"/>
       <c r="X63" s="117"/>
       <c r="AJ63" s="37"/>
-      <c r="AM63" s="106"/>
+      <c r="AM63" s="106" t="str"/>
       <c r="AN63" s="106"/>
       <c r="AO63" s="106"/>
       <c r="AP63" s="106"/>
@@ -62506,7 +63224,7 @@
         <v>0</v>
       </c>
       <c r="AJ64" s="37"/>
-      <c r="AM64" s="106"/>
+      <c r="AM64" s="106" t="str"/>
       <c r="AN64" s="106"/>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
@@ -62606,7 +63324,7 @@
         <v>8.00</v>
       </c>
       <c r="AJ65" s="37"/>
-      <c r="AM65" s="106"/>
+      <c r="AM65" s="106" t="str"/>
       <c r="AN65" s="106"/>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>

</xml_diff>

<commit_message>
everything should work now
</commit_message>
<xml_diff>
--- a/Auslastung.xlsx
+++ b/Auslastung.xlsx
@@ -2276,7 +2276,9 @@
       <c r="AM2" s="1" t="str">
         <v>16.09-22.09.19</v>
       </c>
-      <c r="AN2" s="18"/>
+      <c r="AN2" s="18" t="str">
+        <v>23.09-29.09.19</v>
+      </c>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
       <c r="AQ2" s="108"/>
@@ -2898,7 +2900,9 @@
       <c r="AM8" s="19">
         <v>34.50</v>
       </c>
-      <c r="AN8" s="19"/>
+      <c r="AN8" s="19">
+        <v>34.50</v>
+      </c>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
       <c r="AQ8" s="20"/>
@@ -3023,7 +3027,9 @@
       <c r="AM9" s="19">
         <v>8.50</v>
       </c>
-      <c r="AN9" s="19"/>
+      <c r="AN9" s="19">
+        <v>8.50</v>
+      </c>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
       <c r="AQ9" s="20"/>
@@ -3419,7 +3425,9 @@
       <c r="AM12" s="20">
         <v>1.25</v>
       </c>
-      <c r="AN12" s="20"/>
+      <c r="AN12" s="20">
+        <v>1.25</v>
+      </c>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20"/>
       <c r="AQ12" s="20"/>
@@ -3512,7 +3520,9 @@
       <c r="AM13" s="20">
         <v>11.75</v>
       </c>
-      <c r="AN13" s="20"/>
+      <c r="AN13" s="20">
+        <v>11.75</v>
+      </c>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
       <c r="AQ13" s="20"/>
@@ -3635,7 +3645,9 @@
       <c r="AM14" s="20">
         <v>13.50</v>
       </c>
-      <c r="AN14" s="38"/>
+      <c r="AN14" s="38">
+        <v>13.50</v>
+      </c>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
       <c r="AQ14" s="20"/>
@@ -3762,7 +3774,9 @@
       <c r="AM15" s="20">
         <v>17.50</v>
       </c>
-      <c r="AN15" s="38"/>
+      <c r="AN15" s="38">
+        <v>17.50</v>
+      </c>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
       <c r="AQ15" s="20"/>
@@ -3883,7 +3897,9 @@
       <c r="AM16" s="20">
         <v>13.25</v>
       </c>
-      <c r="AN16" s="38"/>
+      <c r="AN16" s="38">
+        <v>13.25</v>
+      </c>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
       <c r="AQ16" s="20"/>
@@ -4010,7 +4026,9 @@
       <c r="AM17" s="20">
         <v>19.50</v>
       </c>
-      <c r="AN17" s="38"/>
+      <c r="AN17" s="38">
+        <v>19.50</v>
+      </c>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20"/>
       <c r="AQ17" s="20"/>
@@ -4234,7 +4252,9 @@
       <c r="AM19" s="20">
         <v>20.50</v>
       </c>
-      <c r="AN19" s="38"/>
+      <c r="AN19" s="38">
+        <v>20.50</v>
+      </c>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
       <c r="AQ19" s="20"/>
@@ -4359,7 +4379,9 @@
       <c r="AM20" s="37">
         <v>5.75</v>
       </c>
-      <c r="AN20" s="37"/>
+      <c r="AN20" s="37">
+        <v>5.75</v>
+      </c>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
       <c r="AQ20" s="20"/>
@@ -4486,7 +4508,9 @@
       <c r="AM21" s="35">
         <v>25.00</v>
       </c>
-      <c r="AN21" s="35"/>
+      <c r="AN21" s="35">
+        <v>25.00</v>
+      </c>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
       <c r="AQ21" s="37"/>
@@ -4613,7 +4637,9 @@
       <c r="AM22" s="35">
         <v>5.75</v>
       </c>
-      <c r="AN22" s="35"/>
+      <c r="AN22" s="35">
+        <v>5.75</v>
+      </c>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
       <c r="AQ22" s="37"/>
@@ -5011,7 +5037,9 @@
       <c r="AM25" s="19">
         <v>17.00</v>
       </c>
-      <c r="AN25" s="19"/>
+      <c r="AN25" s="19">
+        <v>17.00</v>
+      </c>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
       <c r="AQ25" s="20"/>
@@ -5132,7 +5160,9 @@
       <c r="AM26" s="20">
         <v>13.00</v>
       </c>
-      <c r="AN26" s="38"/>
+      <c r="AN26" s="38">
+        <v>13.00</v>
+      </c>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
       <c r="AQ26" s="20"/>
@@ -5259,7 +5289,9 @@
       <c r="AM27" s="20">
         <v>29.00</v>
       </c>
-      <c r="AN27" s="38"/>
+      <c r="AN27" s="38">
+        <v>29.00</v>
+      </c>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
       <c r="AQ27" s="20"/>
@@ -5374,7 +5406,9 @@
       <c r="AM28" s="20">
         <v>4.75</v>
       </c>
-      <c r="AN28" s="38"/>
+      <c r="AN28" s="38">
+        <v>4.75</v>
+      </c>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
       <c r="AQ28" s="20"/>
@@ -5497,7 +5531,9 @@
       <c r="AM29" s="20">
         <v>19.75</v>
       </c>
-      <c r="AN29" s="38"/>
+      <c r="AN29" s="38">
+        <v>19.75</v>
+      </c>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
       <c r="AQ29" s="20"/>
@@ -5624,7 +5660,9 @@
       <c r="AM30" s="20">
         <v>21.00</v>
       </c>
-      <c r="AN30" s="38"/>
+      <c r="AN30" s="38">
+        <v>21.00</v>
+      </c>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
       <c r="AQ30" s="20"/>
@@ -5866,7 +5904,9 @@
       <c r="AM32" s="20">
         <v>20.50</v>
       </c>
-      <c r="AN32" s="38"/>
+      <c r="AN32" s="38">
+        <v>20.50</v>
+      </c>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
       <c r="AQ32" s="20"/>
@@ -5993,7 +6033,9 @@
       <c r="AM33" s="20">
         <v>14.25</v>
       </c>
-      <c r="AN33" s="38"/>
+      <c r="AN33" s="38">
+        <v>14.25</v>
+      </c>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
       <c r="AQ33" s="37"/>
@@ -6120,7 +6162,9 @@
       <c r="AM34" s="35">
         <v>39.00</v>
       </c>
-      <c r="AN34" s="35"/>
+      <c r="AN34" s="35">
+        <v>39.00</v>
+      </c>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
       <c r="AQ34" s="35"/>
@@ -6247,7 +6291,9 @@
       <c r="AM35" s="35">
         <v>7.00</v>
       </c>
-      <c r="AN35" s="35"/>
+      <c r="AN35" s="35">
+        <v>7.00</v>
+      </c>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
       <c r="AQ35" s="35"/>
@@ -7013,7 +7059,9 @@
       <c r="AM41" s="20">
         <v>2.50</v>
       </c>
-      <c r="AN41" s="38"/>
+      <c r="AN41" s="38">
+        <v>2.50</v>
+      </c>
       <c r="AO41" s="20"/>
       <c r="AP41" s="20"/>
       <c r="AQ41" s="20"/>
@@ -7137,7 +7185,9 @@
       <c r="AM42" s="20">
         <v>22.00</v>
       </c>
-      <c r="AN42" s="38"/>
+      <c r="AN42" s="38">
+        <v>22.00</v>
+      </c>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
       <c r="AQ42" s="20"/>
@@ -7326,7 +7376,9 @@
       <c r="AM44" s="20">
         <v>24.00</v>
       </c>
-      <c r="AN44" s="38"/>
+      <c r="AN44" s="38">
+        <v>24.00</v>
+      </c>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
       <c r="AQ44" s="20"/>
@@ -7534,7 +7586,9 @@
       <c r="AM46" s="37">
         <v>12.00</v>
       </c>
-      <c r="AN46" s="37"/>
+      <c r="AN46" s="37">
+        <v>12.00</v>
+      </c>
       <c r="AO46" s="37"/>
       <c r="AP46" s="37"/>
       <c r="AQ46" s="37"/>
@@ -8203,7 +8257,9 @@
       <c r="AM51" s="20">
         <v>2.25</v>
       </c>
-      <c r="AN51" s="20"/>
+      <c r="AN51" s="20">
+        <v>2.25</v>
+      </c>
       <c r="AO51" s="20"/>
       <c r="AP51" s="20"/>
       <c r="AQ51" s="20"/>
@@ -8326,7 +8382,9 @@
       <c r="AM52" s="20">
         <v>4.75</v>
       </c>
-      <c r="AN52" s="20"/>
+      <c r="AN52" s="20">
+        <v>4.75</v>
+      </c>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
       <c r="AQ52" s="20"/>
@@ -8813,7 +8871,9 @@
       <c r="AM56" s="19">
         <v>8.75</v>
       </c>
-      <c r="AN56" s="37"/>
+      <c r="AN56" s="37">
+        <v>8.75</v>
+      </c>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37"/>
       <c r="BB56" s="23">
@@ -9292,7 +9352,9 @@
       <c r="AM60" s="106">
         <v>25.00</v>
       </c>
-      <c r="AN60" s="106"/>
+      <c r="AN60" s="106">
+        <v>25.00</v>
+      </c>
       <c r="AO60" s="106"/>
       <c r="AP60" s="106"/>
       <c r="AQ60" s="113"/>
@@ -9390,7 +9452,9 @@
       <c r="AM61" s="106">
         <v>4.00</v>
       </c>
-      <c r="AN61" s="106"/>
+      <c r="AN61" s="106">
+        <v>4.00</v>
+      </c>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
       <c r="AQ61" s="113"/>
@@ -9487,7 +9551,9 @@
       <c r="AM62" s="106">
         <v>16.75</v>
       </c>
-      <c r="AN62" s="106"/>
+      <c r="AN62" s="106">
+        <v>16.75</v>
+      </c>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
       <c r="AQ62" s="113"/>
@@ -9681,7 +9747,9 @@
       <c r="AM64" s="106">
         <v>2.00</v>
       </c>
-      <c r="AN64" s="106"/>
+      <c r="AN64" s="106">
+        <v>2.00</v>
+      </c>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
       <c r="AQ64" s="113"/>
@@ -9804,7 +9872,9 @@
       <c r="AM65" s="106">
         <v>20.50</v>
       </c>
-      <c r="AN65" s="106"/>
+      <c r="AN65" s="106">
+        <v>20.50</v>
+      </c>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
       <c r="AQ65" s="113"/>
@@ -11538,7 +11608,9 @@
       <c r="AM2" s="1" t="str">
         <v>16.09-22.09.19</v>
       </c>
-      <c r="AN2" s="18"/>
+      <c r="AN2" s="18" t="str">
+        <v>23.09-29.09.19</v>
+      </c>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
       <c r="AQ2" s="108"/>
@@ -19057,7 +19129,9 @@
       <c r="AM2" s="1" t="str">
         <v>16.09-22.09.19</v>
       </c>
-      <c r="AN2" s="18"/>
+      <c r="AN2" s="18" t="str">
+        <v>23.09-29.09.19</v>
+      </c>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
       <c r="AQ2" s="108"/>
@@ -20340,7 +20414,9 @@
       <c r="AM14" s="20">
         <v>3.00</v>
       </c>
-      <c r="AN14" s="38"/>
+      <c r="AN14" s="38">
+        <v>3.00</v>
+      </c>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
       <c r="AQ14" s="20"/>
@@ -20459,7 +20535,9 @@
       <c r="AM15" s="20">
         <v>5.00</v>
       </c>
-      <c r="AN15" s="38"/>
+      <c r="AN15" s="38">
+        <v>5.00</v>
+      </c>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
       <c r="AQ15" s="20"/>
@@ -20577,7 +20655,9 @@
       <c r="AM16" s="20">
         <v>5.50</v>
       </c>
-      <c r="AN16" s="38"/>
+      <c r="AN16" s="38">
+        <v>5.50</v>
+      </c>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
       <c r="AQ16" s="20"/>
@@ -20908,7 +20988,9 @@
       <c r="AM19" s="20">
         <v>4.00</v>
       </c>
-      <c r="AN19" s="38"/>
+      <c r="AN19" s="38">
+        <v>4.00</v>
+      </c>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
       <c r="AQ19" s="20"/>
@@ -21031,7 +21113,9 @@
       <c r="AM20" s="37">
         <v>7.25</v>
       </c>
-      <c r="AN20" s="37"/>
+      <c r="AN20" s="37">
+        <v>7.25</v>
+      </c>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
       <c r="AQ20" s="20"/>
@@ -21263,7 +21347,9 @@
       <c r="AM22" s="35">
         <v>15.00</v>
       </c>
-      <c r="AN22" s="35"/>
+      <c r="AN22" s="35">
+        <v>15.00</v>
+      </c>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
       <c r="AQ22" s="37"/>
@@ -21884,7 +21970,9 @@
       <c r="AM27" s="20">
         <v>2.75</v>
       </c>
-      <c r="AN27" s="38"/>
+      <c r="AN27" s="38">
+        <v>2.75</v>
+      </c>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
       <c r="AQ27" s="20"/>
@@ -22223,7 +22311,9 @@
       <c r="AM30" s="20">
         <v>0.50</v>
       </c>
-      <c r="AN30" s="38"/>
+      <c r="AN30" s="38">
+        <v>0.50</v>
+      </c>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
       <c r="AQ30" s="20"/>
@@ -22463,7 +22553,9 @@
       <c r="AM32" s="20">
         <v>6.50</v>
       </c>
-      <c r="AN32" s="38"/>
+      <c r="AN32" s="38">
+        <v>6.50</v>
+      </c>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
       <c r="AQ32" s="20"/>
@@ -22590,7 +22682,9 @@
       <c r="AM33" s="20">
         <v>2.25</v>
       </c>
-      <c r="AN33" s="38"/>
+      <c r="AN33" s="38">
+        <v>2.25</v>
+      </c>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
       <c r="AQ33" s="37"/>
@@ -23675,7 +23769,9 @@
       <c r="AM42" s="20">
         <v>7.00</v>
       </c>
-      <c r="AN42" s="38"/>
+      <c r="AN42" s="38">
+        <v>7.00</v>
+      </c>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
       <c r="AQ42" s="20"/>
@@ -23858,7 +23954,9 @@
       <c r="AM44" s="20">
         <v>3.50</v>
       </c>
-      <c r="AN44" s="38"/>
+      <c r="AN44" s="38">
+        <v>3.50</v>
+      </c>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
       <c r="AQ44" s="20"/>
@@ -24815,7 +24913,9 @@
       <c r="AM52" s="20">
         <v>2.25</v>
       </c>
-      <c r="AN52" s="20"/>
+      <c r="AN52" s="20">
+        <v>2.25</v>
+      </c>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
       <c r="AQ52" s="20"/>
@@ -25898,7 +25998,9 @@
       <c r="AM62" s="106">
         <v>0.50</v>
       </c>
-      <c r="AN62" s="106"/>
+      <c r="AN62" s="106">
+        <v>0.50</v>
+      </c>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
       <c r="AQ62" s="113"/>
@@ -26077,7 +26179,9 @@
       <c r="AM64" s="106">
         <v>1.50</v>
       </c>
-      <c r="AN64" s="106"/>
+      <c r="AN64" s="106">
+        <v>1.50</v>
+      </c>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
       <c r="AQ64" s="113"/>
@@ -26182,7 +26286,9 @@
       <c r="AM65" s="106">
         <v>4.00</v>
       </c>
-      <c r="AN65" s="106"/>
+      <c r="AN65" s="106">
+        <v>4.00</v>
+      </c>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
       <c r="AQ65" s="113"/>
@@ -26838,7 +26944,9 @@
       <c r="AM2" s="1" t="str">
         <v>16.09-22.09.19</v>
       </c>
-      <c r="AN2" s="18"/>
+      <c r="AN2" s="18" t="str">
+        <v>23.09-29.09.19</v>
+      </c>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
       <c r="AQ2" s="108"/>
@@ -27450,7 +27558,9 @@
       <c r="AM8" s="19">
         <v>4.75</v>
       </c>
-      <c r="AN8" s="19"/>
+      <c r="AN8" s="19">
+        <v>4.75</v>
+      </c>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
       <c r="AQ8" s="20"/>
@@ -27575,7 +27685,9 @@
       <c r="AM9" s="19">
         <v>31.50</v>
       </c>
-      <c r="AN9" s="19"/>
+      <c r="AN9" s="19">
+        <v>31.50</v>
+      </c>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
       <c r="AQ9" s="20"/>
@@ -27971,7 +28083,9 @@
       <c r="AM12" s="20">
         <v>16.00</v>
       </c>
-      <c r="AN12" s="20"/>
+      <c r="AN12" s="20">
+        <v>16.00</v>
+      </c>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20"/>
       <c r="AQ12" s="20"/>
@@ -28064,7 +28178,9 @@
       <c r="AM13" s="20">
         <v>4.75</v>
       </c>
-      <c r="AN13" s="20"/>
+      <c r="AN13" s="20">
+        <v>4.75</v>
+      </c>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
       <c r="AQ13" s="20"/>
@@ -28188,7 +28304,9 @@
       <c r="AM14" s="20">
         <v>23.50</v>
       </c>
-      <c r="AN14" s="38"/>
+      <c r="AN14" s="38">
+        <v>23.50</v>
+      </c>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20"/>
       <c r="AQ14" s="20"/>
@@ -28315,7 +28433,9 @@
       <c r="AM15" s="20">
         <v>17.50</v>
       </c>
-      <c r="AN15" s="38"/>
+      <c r="AN15" s="38">
+        <v>17.50</v>
+      </c>
       <c r="AO15" s="20"/>
       <c r="AP15" s="20"/>
       <c r="AQ15" s="20"/>
@@ -28436,7 +28556,9 @@
       <c r="AM16" s="20">
         <v>22.25</v>
       </c>
-      <c r="AN16" s="38"/>
+      <c r="AN16" s="38">
+        <v>22.25</v>
+      </c>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20"/>
       <c r="AQ16" s="20"/>
@@ -28563,7 +28685,9 @@
       <c r="AM17" s="20">
         <v>27.50</v>
       </c>
-      <c r="AN17" s="38"/>
+      <c r="AN17" s="38">
+        <v>27.50</v>
+      </c>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20"/>
       <c r="AQ17" s="20"/>
@@ -28787,7 +28911,9 @@
       <c r="AM19" s="20">
         <v>7.25</v>
       </c>
-      <c r="AN19" s="38"/>
+      <c r="AN19" s="38">
+        <v>7.25</v>
+      </c>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
       <c r="AQ19" s="20"/>
@@ -28912,7 +29038,9 @@
       <c r="AM20" s="37">
         <v>32.50</v>
       </c>
-      <c r="AN20" s="37"/>
+      <c r="AN20" s="37">
+        <v>32.50</v>
+      </c>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
       <c r="AQ20" s="20"/>
@@ -29037,7 +29165,9 @@
       <c r="AM21" s="35">
         <v>3.00</v>
       </c>
-      <c r="AN21" s="35"/>
+      <c r="AN21" s="35">
+        <v>3.00</v>
+      </c>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
       <c r="AQ21" s="37"/>
@@ -29164,7 +29294,9 @@
       <c r="AM22" s="35">
         <v>19.00</v>
       </c>
-      <c r="AN22" s="35"/>
+      <c r="AN22" s="35">
+        <v>19.00</v>
+      </c>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
       <c r="AQ22" s="37"/>
@@ -29562,7 +29694,9 @@
       <c r="AM25" s="19">
         <v>23.75</v>
       </c>
-      <c r="AN25" s="19"/>
+      <c r="AN25" s="19">
+        <v>23.75</v>
+      </c>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
       <c r="AQ25" s="20"/>
@@ -29680,7 +29814,9 @@
       <c r="AM26" s="20">
         <v>26.00</v>
       </c>
-      <c r="AN26" s="38"/>
+      <c r="AN26" s="38">
+        <v>26.00</v>
+      </c>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
       <c r="AQ26" s="20"/>
@@ -29805,7 +29941,9 @@
       <c r="AM27" s="20">
         <v>11.00</v>
       </c>
-      <c r="AN27" s="38"/>
+      <c r="AN27" s="38">
+        <v>11.00</v>
+      </c>
       <c r="AO27" s="20"/>
       <c r="AP27" s="20"/>
       <c r="AQ27" s="20"/>
@@ -29920,7 +30058,9 @@
       <c r="AM28" s="20">
         <v>35.25</v>
       </c>
-      <c r="AN28" s="38"/>
+      <c r="AN28" s="38">
+        <v>35.25</v>
+      </c>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
       <c r="AQ28" s="20"/>
@@ -30036,7 +30176,9 @@
       <c r="AM29" s="20">
         <v>4.50</v>
       </c>
-      <c r="AN29" s="38"/>
+      <c r="AN29" s="38">
+        <v>4.50</v>
+      </c>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
       <c r="AQ29" s="20"/>
@@ -30158,7 +30300,9 @@
       <c r="AM30" s="20">
         <v>18.50</v>
       </c>
-      <c r="AN30" s="38"/>
+      <c r="AN30" s="38">
+        <v>18.50</v>
+      </c>
       <c r="AO30" s="20"/>
       <c r="AP30" s="20"/>
       <c r="AQ30" s="20"/>
@@ -30400,7 +30544,9 @@
       <c r="AM32" s="20">
         <v>13.00</v>
       </c>
-      <c r="AN32" s="38"/>
+      <c r="AN32" s="38">
+        <v>13.00</v>
+      </c>
       <c r="AO32" s="20"/>
       <c r="AP32" s="20"/>
       <c r="AQ32" s="20"/>
@@ -30521,7 +30667,9 @@
       <c r="AM33" s="20">
         <v>15.25</v>
       </c>
-      <c r="AN33" s="38"/>
+      <c r="AN33" s="38">
+        <v>15.25</v>
+      </c>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
       <c r="AQ33" s="37"/>
@@ -30646,7 +30794,9 @@
       <c r="AM34" s="35">
         <v>1.00</v>
       </c>
-      <c r="AN34" s="35"/>
+      <c r="AN34" s="35">
+        <v>1.00</v>
+      </c>
       <c r="AO34" s="35"/>
       <c r="AP34" s="35"/>
       <c r="AQ34" s="35"/>
@@ -30773,7 +30923,9 @@
       <c r="AM35" s="35">
         <v>35.00</v>
       </c>
-      <c r="AN35" s="35"/>
+      <c r="AN35" s="35">
+        <v>35.00</v>
+      </c>
       <c r="AO35" s="35"/>
       <c r="AP35" s="35"/>
       <c r="AQ35" s="35"/>
@@ -31539,7 +31691,9 @@
       <c r="AM41" s="20">
         <v>30.00</v>
       </c>
-      <c r="AN41" s="38"/>
+      <c r="AN41" s="38">
+        <v>30.00</v>
+      </c>
       <c r="AO41" s="20"/>
       <c r="AP41" s="20"/>
       <c r="AQ41" s="20"/>
@@ -31662,7 +31816,9 @@
       <c r="AM42" s="20">
         <v>3.00</v>
       </c>
-      <c r="AN42" s="38"/>
+      <c r="AN42" s="38">
+        <v>3.00</v>
+      </c>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20"/>
       <c r="AQ42" s="20"/>
@@ -31847,7 +32003,9 @@
       <c r="AM44" s="20">
         <v>0.75</v>
       </c>
-      <c r="AN44" s="38"/>
+      <c r="AN44" s="38">
+        <v>0.75</v>
+      </c>
       <c r="AO44" s="20"/>
       <c r="AP44" s="20"/>
       <c r="AQ44" s="20"/>
@@ -32050,7 +32208,9 @@
       <c r="AM46" s="37">
         <v>23.00</v>
       </c>
-      <c r="AN46" s="37"/>
+      <c r="AN46" s="37">
+        <v>23.00</v>
+      </c>
       <c r="AO46" s="37"/>
       <c r="AP46" s="37"/>
       <c r="AQ46" s="37"/>
@@ -32721,7 +32881,9 @@
       <c r="AM51" s="20">
         <v>35.75</v>
       </c>
-      <c r="AN51" s="20"/>
+      <c r="AN51" s="20">
+        <v>35.75</v>
+      </c>
       <c r="AO51" s="20"/>
       <c r="AP51" s="20"/>
       <c r="AQ51" s="20"/>
@@ -32844,7 +33006,9 @@
       <c r="AM52" s="20">
         <v>33.00</v>
       </c>
-      <c r="AN52" s="20"/>
+      <c r="AN52" s="20">
+        <v>33.00</v>
+      </c>
       <c r="AO52" s="20"/>
       <c r="AP52" s="20"/>
       <c r="AQ52" s="20"/>
@@ -32967,7 +33131,9 @@
       <c r="AM53" s="20">
         <v>40.00</v>
       </c>
-      <c r="AN53" s="20"/>
+      <c r="AN53" s="20">
+        <v>40.00</v>
+      </c>
       <c r="AO53" s="20"/>
       <c r="AP53" s="20"/>
       <c r="AQ53" s="20"/>
@@ -33347,7 +33513,9 @@
       <c r="AM56" s="19">
         <v>32.75</v>
       </c>
-      <c r="AN56" s="37"/>
+      <c r="AN56" s="37">
+        <v>32.75</v>
+      </c>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37"/>
       <c r="BB56" s="23">
@@ -33822,7 +33990,9 @@
       <c r="AM60" s="106">
         <v>10.00</v>
       </c>
-      <c r="AN60" s="106"/>
+      <c r="AN60" s="106">
+        <v>10.00</v>
+      </c>
       <c r="AO60" s="106"/>
       <c r="AP60" s="106"/>
       <c r="AQ60" s="113"/>
@@ -33920,7 +34090,9 @@
       <c r="AM61" s="106">
         <v>20.00</v>
       </c>
-      <c r="AN61" s="106"/>
+      <c r="AN61" s="106">
+        <v>20.00</v>
+      </c>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
       <c r="AQ61" s="113"/>
@@ -34014,7 +34186,9 @@
       <c r="AM62" s="106">
         <v>18.50</v>
       </c>
-      <c r="AN62" s="106"/>
+      <c r="AN62" s="106">
+        <v>18.50</v>
+      </c>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
       <c r="AQ62" s="113"/>
@@ -34210,7 +34384,9 @@
       <c r="AM64" s="106">
         <v>25.50</v>
       </c>
-      <c r="AN64" s="106"/>
+      <c r="AN64" s="106">
+        <v>25.50</v>
+      </c>
       <c r="AO64" s="106"/>
       <c r="AP64" s="106"/>
       <c r="AQ64" s="113"/>
@@ -34333,7 +34509,9 @@
       <c r="AM65" s="106">
         <v>15.00</v>
       </c>
-      <c r="AN65" s="106"/>
+      <c r="AN65" s="106">
+        <v>15.00</v>
+      </c>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
       <c r="AQ65" s="113"/>
@@ -34988,7 +35166,9 @@
       <c r="AM2" s="1" t="str">
         <v>16.09-22.09.19</v>
       </c>
-      <c r="AN2" s="18"/>
+      <c r="AN2" s="18" t="str">
+        <v>23.09-29.09.19</v>
+      </c>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
       <c r="AQ2" s="108"/>
@@ -36160,7 +36340,9 @@
       <c r="AM13" s="20">
         <v>24.00</v>
       </c>
-      <c r="AN13" s="20"/>
+      <c r="AN13" s="20">
+        <v>24.00</v>
+      </c>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20"/>
       <c r="AQ13" s="20"/>
@@ -36815,7 +36997,9 @@
       <c r="AM19" s="20">
         <v>8.00</v>
       </c>
-      <c r="AN19" s="38"/>
+      <c r="AN19" s="38">
+        <v>8.00</v>
+      </c>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20"/>
       <c r="AQ19" s="20"/>
@@ -36936,7 +37120,9 @@
       <c r="AM20" s="37">
         <v>4.00</v>
       </c>
-      <c r="AN20" s="37"/>
+      <c r="AN20" s="37">
+        <v>4.00</v>
+      </c>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20"/>
       <c r="AQ20" s="20"/>
@@ -37051,7 +37237,9 @@
       <c r="AM21" s="35">
         <v>7.00</v>
       </c>
-      <c r="AN21" s="35"/>
+      <c r="AN21" s="35">
+        <v>7.00</v>
+      </c>
       <c r="AO21" s="35"/>
       <c r="AP21" s="37"/>
       <c r="AQ21" s="37"/>
@@ -37988,7 +38176,9 @@
       <c r="AM29" s="20">
         <v>5.00</v>
       </c>
-      <c r="AN29" s="38"/>
+      <c r="AN29" s="38">
+        <v>5.00</v>
+      </c>
       <c r="AO29" s="20"/>
       <c r="AP29" s="20"/>
       <c r="AQ29" s="20"/>
@@ -38215,7 +38405,9 @@
       <c r="AM31" s="20">
         <v>40.00</v>
       </c>
-      <c r="AN31" s="38"/>
+      <c r="AN31" s="38">
+        <v>40.00</v>
+      </c>
       <c r="AO31" s="20"/>
       <c r="AP31" s="20"/>
       <c r="AQ31" s="20"/>
@@ -38441,7 +38633,9 @@
       <c r="AM33" s="20">
         <v>8.00</v>
       </c>
-      <c r="AN33" s="38"/>
+      <c r="AN33" s="38">
+        <v>8.00</v>
+      </c>
       <c r="AO33" s="37"/>
       <c r="AP33" s="20"/>
       <c r="AQ33" s="37"/>
@@ -41681,7 +41875,9 @@
       <c r="AM61" s="106">
         <v>16.00</v>
       </c>
-      <c r="AN61" s="106"/>
+      <c r="AN61" s="106">
+        <v>16.00</v>
+      </c>
       <c r="AO61" s="106"/>
       <c r="AP61" s="106"/>
       <c r="AQ61" s="113"/>
@@ -41757,7 +41953,9 @@
       <c r="AM62" s="106">
         <v>4.00</v>
       </c>
-      <c r="AN62" s="106"/>
+      <c r="AN62" s="106">
+        <v>4.00</v>
+      </c>
       <c r="AO62" s="106"/>
       <c r="AP62" s="106"/>
       <c r="AQ62" s="113"/>
@@ -42677,7 +42875,9 @@
       <c r="AM2" s="1" t="str">
         <v>16.09-22.09.19</v>
       </c>
-      <c r="AN2" s="18"/>
+      <c r="AN2" s="18" t="str">
+        <v>23.09-29.09.19</v>
+      </c>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
       <c r="AQ2" s="108"/>
@@ -44815,7 +45015,9 @@
       <c r="AM22" s="35">
         <v>0.25</v>
       </c>
-      <c r="AN22" s="35"/>
+      <c r="AN22" s="35">
+        <v>0.25</v>
+      </c>
       <c r="AO22" s="35"/>
       <c r="AP22" s="37"/>
       <c r="AQ22" s="37"/>
@@ -45311,7 +45513,9 @@
       <c r="AM26" s="20">
         <v>1.00</v>
       </c>
-      <c r="AN26" s="38"/>
+      <c r="AN26" s="38">
+        <v>1.00</v>
+      </c>
       <c r="AO26" s="20"/>
       <c r="AP26" s="20"/>
       <c r="AQ26" s="20"/>
@@ -49608,7 +49812,9 @@
       <c r="AM65" s="106">
         <v>0.50</v>
       </c>
-      <c r="AN65" s="106"/>
+      <c r="AN65" s="106">
+        <v>0.50</v>
+      </c>
       <c r="AO65" s="106"/>
       <c r="AP65" s="106"/>
       <c r="AQ65" s="113"/>
@@ -50265,7 +50471,9 @@
       <c r="AM2" s="1" t="str">
         <v>16.09-22.09.19</v>
       </c>
-      <c r="AN2" s="18"/>
+      <c r="AN2" s="18" t="str">
+        <v>23.09-29.09.19</v>
+      </c>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
       <c r="AQ2" s="108"/>
@@ -56475,7 +56683,9 @@
       <c r="AM2" s="1" t="str">
         <v>16.09-22.09.19</v>
       </c>
-      <c r="AN2" s="18"/>
+      <c r="AN2" s="18" t="str">
+        <v>23.09-29.09.19</v>
+      </c>
       <c r="AO2" s="18"/>
       <c r="AP2" s="18"/>
       <c r="AQ2" s="108"/>

</xml_diff>